<commit_message>
entered May 2016 CAAU data
</commit_message>
<xml_diff>
--- a/caau_monitoring_2016_PI_shared.xlsx
+++ b/caau_monitoring_2016_PI_shared.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh_adams\josh_IBM\CAAU\caau_breeding\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekelsey\Documents\WERC-SC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8256"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Data codes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="168">
   <si>
     <t>Date</t>
   </si>
@@ -343,6 +343,192 @@
   </si>
   <si>
     <t>AD = ADULT</t>
+  </si>
+  <si>
+    <t>EMPTRY</t>
+  </si>
+  <si>
+    <t>ALMOST DEAD, COVERED IN LITTLE RED BUGS, DIDN'T PROCESS</t>
+  </si>
+  <si>
+    <t>1643-03615</t>
+  </si>
+  <si>
+    <t>TUNNEL DETACHED, BOX MOSTLY ERRODED OUT</t>
+  </si>
+  <si>
+    <t>1643-03651</t>
+  </si>
+  <si>
+    <t>1643-03614</t>
+  </si>
+  <si>
+    <t>1313-46069</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>DEAD CHICK TOO</t>
+  </si>
+  <si>
+    <t>1643-03613</t>
+  </si>
+  <si>
+    <t>1643-03641</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>1643-03645</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>1643-03652</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>1643-03642</t>
+  </si>
+  <si>
+    <t>1643-03647</t>
+  </si>
+  <si>
+    <t>BURROWED THROUGH</t>
+  </si>
+  <si>
+    <t>1643-03644</t>
+  </si>
+  <si>
+    <t>1643-03648</t>
+  </si>
+  <si>
+    <t>1643-03649</t>
+  </si>
+  <si>
+    <t>1643-03640</t>
+  </si>
+  <si>
+    <t>1643-03631</t>
+  </si>
+  <si>
+    <t>1643-03612</t>
+  </si>
+  <si>
+    <t>1643-03639</t>
+  </si>
+  <si>
+    <t>1643-03634</t>
+  </si>
+  <si>
+    <t>1643-03636</t>
+  </si>
+  <si>
+    <t>1643-03635</t>
+  </si>
+  <si>
+    <t>1643-03638</t>
+  </si>
+  <si>
+    <t>1643-03637</t>
+  </si>
+  <si>
+    <t>1643-03633</t>
+  </si>
+  <si>
+    <t>EGG SHELL FRAGEMENTS, BURROWED THROUGH</t>
+  </si>
+  <si>
+    <t>1643-03616</t>
+  </si>
+  <si>
+    <t>1643-03618</t>
+  </si>
+  <si>
+    <t>1643-03617</t>
+  </si>
+  <si>
+    <t>1643-03619</t>
+  </si>
+  <si>
+    <t>1643-03650</t>
+  </si>
+  <si>
+    <t>1313-45912</t>
+  </si>
+  <si>
+    <t>1643-03643</t>
+  </si>
+  <si>
+    <t>1643-03646</t>
+  </si>
+  <si>
+    <t>NR</t>
+  </si>
+  <si>
+    <t>1643-03632</t>
+  </si>
+  <si>
+    <t>1643-03630</t>
+  </si>
+  <si>
+    <t>ESCAPED</t>
+  </si>
+  <si>
+    <t>1643-03629</t>
+  </si>
+  <si>
+    <t>1643-10423</t>
+  </si>
+  <si>
+    <t>P1 FEATHERS HADN'T BURST YET</t>
+  </si>
+  <si>
+    <t>1643-03628</t>
+  </si>
+  <si>
+    <t>1643-03627</t>
+  </si>
+  <si>
+    <t>1313-90001</t>
+  </si>
+  <si>
+    <t>1643-03626</t>
+  </si>
+  <si>
+    <t>1643-03625</t>
+  </si>
+  <si>
+    <t>1643-03624</t>
+  </si>
+  <si>
+    <t>1643-03622</t>
+  </si>
+  <si>
+    <t>1313-80091</t>
+  </si>
+  <si>
+    <t>NEWLY-HATCHED CHICK SIZED, PRETTY FRESH</t>
+  </si>
+  <si>
+    <t>LCG</t>
+  </si>
+  <si>
+    <t>1643-03623</t>
+  </si>
+  <si>
+    <t>1643-03621</t>
+  </si>
+  <si>
+    <t>1643-03620</t>
+  </si>
+  <si>
+    <t>1643-10414</t>
   </si>
 </sst>
 </file>
@@ -353,7 +539,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -390,6 +576,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -440,7 +632,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -520,6 +712,13 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -802,15 +1001,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y103"/>
+  <dimension ref="A1:Y174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="I106" sqref="I106"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A141" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R174" sqref="R174"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="7" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -876,7 +1079,7 @@
       </c>
       <c r="V1" s="5"/>
     </row>
-    <row r="2" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>42173</v>
       </c>
@@ -909,7 +1112,7 @@
       <c r="X2" s="12"/>
       <c r="Y2" s="12"/>
     </row>
-    <row r="3" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>42173</v>
       </c>
@@ -942,7 +1145,7 @@
       <c r="X3" s="12"/>
       <c r="Y3" s="12"/>
     </row>
-    <row r="4" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>42173</v>
       </c>
@@ -975,7 +1178,7 @@
       <c r="X4" s="12"/>
       <c r="Y4" s="12"/>
     </row>
-    <row r="5" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>42173</v>
       </c>
@@ -1008,7 +1211,7 @@
       <c r="X5" s="12"/>
       <c r="Y5" s="12"/>
     </row>
-    <row r="6" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>42173</v>
       </c>
@@ -1041,7 +1244,7 @@
       <c r="X6" s="12"/>
       <c r="Y6" s="12"/>
     </row>
-    <row r="7" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>42173</v>
       </c>
@@ -1074,7 +1277,7 @@
       <c r="X7" s="12"/>
       <c r="Y7" s="12"/>
     </row>
-    <row r="8" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>42173</v>
       </c>
@@ -1107,7 +1310,7 @@
       <c r="X8" s="12"/>
       <c r="Y8" s="12"/>
     </row>
-    <row r="9" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>42173</v>
       </c>
@@ -1140,7 +1343,7 @@
       <c r="X9" s="12"/>
       <c r="Y9" s="12"/>
     </row>
-    <row r="10" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>42173</v>
       </c>
@@ -1175,7 +1378,7 @@
       <c r="X10" s="12"/>
       <c r="Y10" s="12"/>
     </row>
-    <row r="11" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>42198</v>
       </c>
@@ -1214,7 +1417,7 @@
       <c r="X11" s="12"/>
       <c r="Y11" s="12"/>
     </row>
-    <row r="12" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>42173</v>
       </c>
@@ -1261,7 +1464,7 @@
       <c r="X12" s="12"/>
       <c r="Y12" s="12"/>
     </row>
-    <row r="13" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>42198</v>
       </c>
@@ -1315,7 +1518,7 @@
       <c r="X13" s="12"/>
       <c r="Y13" s="12"/>
     </row>
-    <row r="14" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>42173</v>
       </c>
@@ -1348,7 +1551,7 @@
       <c r="X14" s="12"/>
       <c r="Y14" s="12"/>
     </row>
-    <row r="15" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>42173</v>
       </c>
@@ -1383,7 +1586,7 @@
       <c r="X15" s="12"/>
       <c r="Y15" s="12"/>
     </row>
-    <row r="16" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>42198</v>
       </c>
@@ -1422,7 +1625,7 @@
       <c r="X16" s="12"/>
       <c r="Y16" s="12"/>
     </row>
-    <row r="17" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>42173</v>
       </c>
@@ -1457,7 +1660,7 @@
       <c r="X17" s="12"/>
       <c r="Y17" s="12"/>
     </row>
-    <row r="18" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>42173</v>
       </c>
@@ -1504,7 +1707,7 @@
       <c r="X18" s="12"/>
       <c r="Y18" s="12"/>
     </row>
-    <row r="19" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>42198</v>
       </c>
@@ -1558,7 +1761,7 @@
       <c r="X19" s="12"/>
       <c r="Y19" s="12"/>
     </row>
-    <row r="20" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>42173</v>
       </c>
@@ -1593,7 +1796,7 @@
       <c r="X20" s="12"/>
       <c r="Y20" s="12"/>
     </row>
-    <row r="21" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>42173</v>
       </c>
@@ -1630,7 +1833,7 @@
       <c r="X21" s="12"/>
       <c r="Y21" s="12"/>
     </row>
-    <row r="22" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>42198</v>
       </c>
@@ -1669,7 +1872,7 @@
       <c r="X22" s="12"/>
       <c r="Y22" s="12"/>
     </row>
-    <row r="23" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>42173</v>
       </c>
@@ -1704,7 +1907,7 @@
       <c r="X23" s="12"/>
       <c r="Y23" s="12"/>
     </row>
-    <row r="24" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>42173</v>
       </c>
@@ -1739,7 +1942,7 @@
       <c r="X24" s="12"/>
       <c r="Y24" s="12"/>
     </row>
-    <row r="25" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>42173</v>
       </c>
@@ -1776,7 +1979,7 @@
       <c r="X25" s="12"/>
       <c r="Y25" s="12"/>
     </row>
-    <row r="26" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>42198</v>
       </c>
@@ -1817,7 +2020,7 @@
       <c r="X26" s="12"/>
       <c r="Y26" s="12"/>
     </row>
-    <row r="27" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>42173</v>
       </c>
@@ -1852,7 +2055,7 @@
       <c r="X27" s="12"/>
       <c r="Y27" s="12"/>
     </row>
-    <row r="28" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>42173</v>
       </c>
@@ -1887,7 +2090,7 @@
       <c r="X28" s="12"/>
       <c r="Y28" s="12"/>
     </row>
-    <row r="29" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>42173</v>
       </c>
@@ -1922,7 +2125,7 @@
       <c r="X29" s="12"/>
       <c r="Y29" s="12"/>
     </row>
-    <row r="30" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>42173</v>
       </c>
@@ -1959,7 +2162,7 @@
       <c r="X30" s="12"/>
       <c r="Y30" s="12"/>
     </row>
-    <row r="31" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>42198</v>
       </c>
@@ -1998,7 +2201,7 @@
       <c r="X31" s="12"/>
       <c r="Y31" s="12"/>
     </row>
-    <row r="32" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>42173</v>
       </c>
@@ -2035,7 +2238,7 @@
       <c r="X32" s="12"/>
       <c r="Y32" s="12"/>
     </row>
-    <row r="33" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>42198</v>
       </c>
@@ -2074,7 +2277,7 @@
       <c r="X33" s="12"/>
       <c r="Y33" s="12"/>
     </row>
-    <row r="34" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>42173</v>
       </c>
@@ -2129,7 +2332,7 @@
       <c r="X34" s="12"/>
       <c r="Y34" s="12"/>
     </row>
-    <row r="35" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>42198</v>
       </c>
@@ -2168,7 +2371,7 @@
       <c r="X35" s="12"/>
       <c r="Y35" s="12"/>
     </row>
-    <row r="36" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
         <v>42173</v>
       </c>
@@ -2203,7 +2406,7 @@
       <c r="X36" s="12"/>
       <c r="Y36" s="12"/>
     </row>
-    <row r="37" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>42173</v>
       </c>
@@ -2238,7 +2441,7 @@
       <c r="X37" s="12"/>
       <c r="Y37" s="12"/>
     </row>
-    <row r="38" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
         <v>42173</v>
       </c>
@@ -2290,7 +2493,7 @@
       <c r="X38" s="12"/>
       <c r="Y38" s="12"/>
     </row>
-    <row r="39" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>42198</v>
       </c>
@@ -2331,7 +2534,7 @@
       <c r="X39" s="12"/>
       <c r="Y39" s="12"/>
     </row>
-    <row r="40" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13">
         <v>42173</v>
       </c>
@@ -2366,7 +2569,7 @@
       <c r="X40" s="12"/>
       <c r="Y40" s="12"/>
     </row>
-    <row r="41" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13">
         <v>42173</v>
       </c>
@@ -2401,7 +2604,7 @@
       <c r="X41" s="12"/>
       <c r="Y41" s="12"/>
     </row>
-    <row r="42" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13">
         <v>42173</v>
       </c>
@@ -2453,7 +2656,7 @@
       <c r="X42" s="12"/>
       <c r="Y42" s="12"/>
     </row>
-    <row r="43" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>42198</v>
       </c>
@@ -2492,7 +2695,7 @@
       <c r="X43" s="12"/>
       <c r="Y43" s="12"/>
     </row>
-    <row r="44" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
         <v>42173</v>
       </c>
@@ -2544,7 +2747,7 @@
       <c r="X44" s="12"/>
       <c r="Y44" s="12"/>
     </row>
-    <row r="45" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>42198</v>
       </c>
@@ -2583,7 +2786,7 @@
       <c r="X45" s="12"/>
       <c r="Y45" s="12"/>
     </row>
-    <row r="46" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="13">
         <v>42173</v>
       </c>
@@ -2620,7 +2823,7 @@
       <c r="X46" s="12"/>
       <c r="Y46" s="12"/>
     </row>
-    <row r="47" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>42198</v>
       </c>
@@ -2659,7 +2862,7 @@
       <c r="X47" s="12"/>
       <c r="Y47" s="12"/>
     </row>
-    <row r="48" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
         <v>42173</v>
       </c>
@@ -2694,7 +2897,7 @@
       <c r="X48" s="12"/>
       <c r="Y48" s="12"/>
     </row>
-    <row r="49" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
         <v>42173</v>
       </c>
@@ -2731,7 +2934,7 @@
       <c r="X49" s="12"/>
       <c r="Y49" s="12"/>
     </row>
-    <row r="50" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>42198</v>
       </c>
@@ -2770,7 +2973,7 @@
       <c r="X50" s="12"/>
       <c r="Y50" s="12"/>
     </row>
-    <row r="51" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="13">
         <v>42173</v>
       </c>
@@ -2822,7 +3025,7 @@
       <c r="X51" s="12"/>
       <c r="Y51" s="12"/>
     </row>
-    <row r="52" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="13">
         <v>42173</v>
       </c>
@@ -2861,7 +3064,7 @@
       <c r="X52" s="12"/>
       <c r="Y52" s="12"/>
     </row>
-    <row r="53" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="21">
         <v>42198</v>
       </c>
@@ -2904,7 +3107,7 @@
       <c r="X53" s="12"/>
       <c r="Y53" s="12"/>
     </row>
-    <row r="54" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="13">
         <v>42173</v>
       </c>
@@ -2939,7 +3142,7 @@
       <c r="X54" s="12"/>
       <c r="Y54" s="12"/>
     </row>
-    <row r="55" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="13">
         <v>42173</v>
       </c>
@@ -2974,7 +3177,7 @@
       <c r="X55" s="12"/>
       <c r="Y55" s="12"/>
     </row>
-    <row r="56" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="13">
         <v>42173</v>
       </c>
@@ -3023,7 +3226,7 @@
       <c r="X56" s="12"/>
       <c r="Y56" s="12"/>
     </row>
-    <row r="57" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>42198</v>
       </c>
@@ -3073,7 +3276,7 @@
       <c r="X57" s="12"/>
       <c r="Y57" s="12"/>
     </row>
-    <row r="58" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="13">
         <v>42173</v>
       </c>
@@ -3110,7 +3313,7 @@
       <c r="X58" s="12"/>
       <c r="Y58" s="12"/>
     </row>
-    <row r="59" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <v>42198</v>
       </c>
@@ -3149,7 +3352,7 @@
       <c r="X59" s="12"/>
       <c r="Y59" s="12"/>
     </row>
-    <row r="60" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="13">
         <v>42173</v>
       </c>
@@ -3201,7 +3404,7 @@
       <c r="X60" s="12"/>
       <c r="Y60" s="12"/>
     </row>
-    <row r="61" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <v>42198</v>
       </c>
@@ -3251,7 +3454,7 @@
       <c r="X61" s="12"/>
       <c r="Y61" s="12"/>
     </row>
-    <row r="62" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="13">
         <v>42173</v>
       </c>
@@ -3286,7 +3489,7 @@
       <c r="X62" s="12"/>
       <c r="Y62" s="12"/>
     </row>
-    <row r="63" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="13">
         <v>42173</v>
       </c>
@@ -3321,7 +3524,7 @@
       <c r="X63" s="12"/>
       <c r="Y63" s="12"/>
     </row>
-    <row r="64" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="13">
         <v>42173</v>
       </c>
@@ -3356,7 +3559,7 @@
       <c r="X64" s="12"/>
       <c r="Y64" s="12"/>
     </row>
-    <row r="65" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="13">
         <v>42173</v>
       </c>
@@ -3408,7 +3611,7 @@
       <c r="X65" s="12"/>
       <c r="Y65" s="12"/>
     </row>
-    <row r="66" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="8">
         <v>42198</v>
       </c>
@@ -3462,7 +3665,7 @@
       <c r="X66" s="12"/>
       <c r="Y66" s="12"/>
     </row>
-    <row r="67" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="13">
         <v>42173</v>
       </c>
@@ -3497,7 +3700,7 @@
       <c r="X67" s="12"/>
       <c r="Y67" s="12"/>
     </row>
-    <row r="68" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="13">
         <v>42173</v>
       </c>
@@ -3532,7 +3735,7 @@
       <c r="X68" s="12"/>
       <c r="Y68" s="12"/>
     </row>
-    <row r="69" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="13">
         <v>42173</v>
       </c>
@@ -3567,7 +3770,7 @@
       <c r="X69" s="12"/>
       <c r="Y69" s="12"/>
     </row>
-    <row r="70" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="13">
         <v>42173</v>
       </c>
@@ -3602,7 +3805,7 @@
       <c r="X70" s="12"/>
       <c r="Y70" s="12"/>
     </row>
-    <row r="71" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="13">
         <v>42173</v>
       </c>
@@ -3637,7 +3840,7 @@
       <c r="X71" s="12"/>
       <c r="Y71" s="12"/>
     </row>
-    <row r="72" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="13">
         <v>42173</v>
       </c>
@@ -3686,7 +3889,7 @@
       <c r="X72" s="12"/>
       <c r="Y72" s="12"/>
     </row>
-    <row r="73" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="8">
         <v>42198</v>
       </c>
@@ -3725,7 +3928,7 @@
       <c r="X73" s="12"/>
       <c r="Y73" s="12"/>
     </row>
-    <row r="74" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="13">
         <v>42173</v>
       </c>
@@ -3762,7 +3965,7 @@
       <c r="X74" s="12"/>
       <c r="Y74" s="12"/>
     </row>
-    <row r="75" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="13">
         <v>42173</v>
       </c>
@@ -3799,7 +4002,7 @@
       <c r="X75" s="12"/>
       <c r="Y75" s="12"/>
     </row>
-    <row r="76" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="13">
         <v>42173</v>
       </c>
@@ -3853,7 +4056,7 @@
       <c r="X76" s="12"/>
       <c r="Y76" s="12"/>
     </row>
-    <row r="77" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="8">
         <v>42198</v>
       </c>
@@ -3892,7 +4095,7 @@
       <c r="X77" s="12"/>
       <c r="Y77" s="12"/>
     </row>
-    <row r="78" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="13">
         <v>42173</v>
       </c>
@@ -3931,7 +4134,7 @@
       <c r="X78" s="12"/>
       <c r="Y78" s="12"/>
     </row>
-    <row r="79" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="13">
         <v>42173</v>
       </c>
@@ -3970,7 +4173,7 @@
       <c r="X79" s="12"/>
       <c r="Y79" s="12"/>
     </row>
-    <row r="80" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="13">
         <v>42173</v>
       </c>
@@ -4009,7 +4212,7 @@
       <c r="X80" s="12"/>
       <c r="Y80" s="12"/>
     </row>
-    <row r="81" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="13">
         <v>42173</v>
       </c>
@@ -4048,7 +4251,7 @@
       <c r="X81" s="12"/>
       <c r="Y81" s="12"/>
     </row>
-    <row r="82" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="13">
         <v>42173</v>
       </c>
@@ -4087,7 +4290,7 @@
       <c r="X82" s="12"/>
       <c r="Y82" s="12"/>
     </row>
-    <row r="83" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="13">
         <v>42173</v>
       </c>
@@ -4130,7 +4333,7 @@
       <c r="X83" s="12"/>
       <c r="Y83" s="12"/>
     </row>
-    <row r="84" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="8">
         <v>42198</v>
       </c>
@@ -4184,7 +4387,7 @@
       <c r="X84" s="12"/>
       <c r="Y84" s="12"/>
     </row>
-    <row r="85" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="13">
         <v>42173</v>
       </c>
@@ -4223,7 +4426,7 @@
       <c r="X85" s="12"/>
       <c r="Y85" s="12"/>
     </row>
-    <row r="86" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="13">
         <v>42173</v>
       </c>
@@ -4264,7 +4467,7 @@
       <c r="X86" s="12"/>
       <c r="Y86" s="12"/>
     </row>
-    <row r="87" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="8">
         <v>42198</v>
       </c>
@@ -4303,7 +4506,7 @@
       <c r="X87" s="12"/>
       <c r="Y87" s="12"/>
     </row>
-    <row r="88" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="13">
         <v>42173</v>
       </c>
@@ -4344,7 +4547,7 @@
       <c r="X88" s="12"/>
       <c r="Y88" s="12"/>
     </row>
-    <row r="89" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="8">
         <v>42198</v>
       </c>
@@ -4383,7 +4586,7 @@
       <c r="X89" s="12"/>
       <c r="Y89" s="12"/>
     </row>
-    <row r="90" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="13">
         <v>42173</v>
       </c>
@@ -4424,7 +4627,7 @@
       <c r="X90" s="12"/>
       <c r="Y90" s="12"/>
     </row>
-    <row r="91" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="8">
         <v>42198</v>
       </c>
@@ -4463,7 +4666,7 @@
       <c r="X91" s="12"/>
       <c r="Y91" s="12"/>
     </row>
-    <row r="92" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="13">
         <v>42173</v>
       </c>
@@ -4502,7 +4705,7 @@
       <c r="X92" s="12"/>
       <c r="Y92" s="12"/>
     </row>
-    <row r="93" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="13">
         <v>42173</v>
       </c>
@@ -4541,7 +4744,7 @@
       <c r="X93" s="12"/>
       <c r="Y93" s="12"/>
     </row>
-    <row r="94" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="13">
         <v>42173</v>
       </c>
@@ -4580,7 +4783,7 @@
       <c r="X94" s="12"/>
       <c r="Y94" s="12"/>
     </row>
-    <row r="95" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="8">
         <v>42198</v>
       </c>
@@ -4621,7 +4824,7 @@
       <c r="X95" s="12"/>
       <c r="Y95" s="12"/>
     </row>
-    <row r="96" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="13">
         <v>42173</v>
       </c>
@@ -4662,7 +4865,7 @@
       <c r="X96" s="12"/>
       <c r="Y96" s="12"/>
     </row>
-    <row r="97" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="8">
         <v>42198</v>
       </c>
@@ -4701,7 +4904,7 @@
       <c r="X97" s="12"/>
       <c r="Y97" s="12"/>
     </row>
-    <row r="98" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="13">
         <v>42173</v>
       </c>
@@ -4755,7 +4958,7 @@
       <c r="X98" s="12"/>
       <c r="Y98" s="12"/>
     </row>
-    <row r="99" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="8">
         <v>42198</v>
       </c>
@@ -4794,7 +4997,7 @@
       <c r="X99" s="12"/>
       <c r="Y99" s="12"/>
     </row>
-    <row r="100" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="13">
         <v>42173</v>
       </c>
@@ -4833,7 +5036,7 @@
       <c r="X100" s="12"/>
       <c r="Y100" s="12"/>
     </row>
-    <row r="101" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="13">
         <v>42173</v>
       </c>
@@ -4872,7 +5075,7 @@
       <c r="X101" s="12"/>
       <c r="Y101" s="12"/>
     </row>
-    <row r="102" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="13">
         <v>42173</v>
       </c>
@@ -4911,11 +5114,2604 @@
       <c r="X102" s="12"/>
       <c r="Y102" s="12"/>
     </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A103" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B103" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C103" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D103" s="11">
+        <v>1</v>
+      </c>
+      <c r="E103" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H103" s="15" t="s">
+        <v>106</v>
+      </c>
       <c r="Q103" s="12">
         <f>O103-P103</f>
         <v>0</v>
       </c>
+    </row>
+    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A104" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B104" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C104" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D104" s="11">
+        <v>2</v>
+      </c>
+      <c r="E104" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G104" t="s">
+        <v>26</v>
+      </c>
+      <c r="H104" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="U104" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A105" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B105" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C105" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D105" s="11">
+        <v>3</v>
+      </c>
+      <c r="E105" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G105" t="s">
+        <v>26</v>
+      </c>
+      <c r="H105" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I105" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="M105">
+        <v>96</v>
+      </c>
+      <c r="N105">
+        <v>50</v>
+      </c>
+      <c r="O105">
+        <v>150</v>
+      </c>
+      <c r="P105">
+        <v>14</v>
+      </c>
+      <c r="Q105">
+        <f>O105-P105</f>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A106" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B106" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C106" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D106" s="11">
+        <v>4</v>
+      </c>
+      <c r="E106" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H106" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="U106" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A107" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B107" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C107" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D107" s="11">
+        <v>5</v>
+      </c>
+      <c r="E107" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H107" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A108" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B108" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C108" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D108" s="11">
+        <v>6</v>
+      </c>
+      <c r="E108" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G108" t="s">
+        <v>26</v>
+      </c>
+      <c r="H108" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I108" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="M108">
+        <v>104</v>
+      </c>
+      <c r="N108">
+        <v>51</v>
+      </c>
+      <c r="O108">
+        <v>178</v>
+      </c>
+      <c r="P108">
+        <v>14</v>
+      </c>
+      <c r="Q108">
+        <f t="shared" ref="Q108:Q148" si="0">O108-P108</f>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A109" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B109" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C109" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D109" s="11">
+        <v>7</v>
+      </c>
+      <c r="E109" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H109" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="110" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A110" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B110" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C110" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D110" s="11">
+        <v>8</v>
+      </c>
+      <c r="E110" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G110" t="s">
+        <v>26</v>
+      </c>
+      <c r="H110" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I110" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="M110">
+        <v>101</v>
+      </c>
+      <c r="N110">
+        <v>48</v>
+      </c>
+      <c r="O110">
+        <v>155</v>
+      </c>
+      <c r="P110">
+        <v>14</v>
+      </c>
+      <c r="Q110">
+        <f t="shared" si="0"/>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="111" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A111" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B111" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C111" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D111" s="11">
+        <v>9</v>
+      </c>
+      <c r="E111" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G111" t="s">
+        <v>37</v>
+      </c>
+      <c r="H111" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I111" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="K111" t="s">
+        <v>113</v>
+      </c>
+      <c r="L111">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="O111">
+        <v>172</v>
+      </c>
+      <c r="P111">
+        <v>14</v>
+      </c>
+      <c r="Q111">
+        <f t="shared" si="0"/>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A112" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B112" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C112" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D112" s="17">
+        <v>10</v>
+      </c>
+      <c r="E112" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G112" t="s">
+        <v>37</v>
+      </c>
+      <c r="H112" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I112" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="K112" t="s">
+        <v>113</v>
+      </c>
+      <c r="L112">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="O112">
+        <v>188</v>
+      </c>
+      <c r="P112">
+        <v>14</v>
+      </c>
+      <c r="Q112">
+        <f t="shared" si="0"/>
+        <v>174</v>
+      </c>
+      <c r="U112" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A113" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B113" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C113" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D113" s="11">
+        <v>11</v>
+      </c>
+      <c r="E113" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G113" t="s">
+        <v>37</v>
+      </c>
+      <c r="H113" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I113" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="K113" t="s">
+        <v>117</v>
+      </c>
+      <c r="L113">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="O113">
+        <v>176</v>
+      </c>
+      <c r="P113">
+        <v>14</v>
+      </c>
+      <c r="Q113">
+        <f t="shared" si="0"/>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A114" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B114" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C114" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D114" s="11">
+        <v>12</v>
+      </c>
+      <c r="E114" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G114" t="s">
+        <v>26</v>
+      </c>
+      <c r="H114" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="M114">
+        <v>37</v>
+      </c>
+      <c r="N114">
+        <v>9</v>
+      </c>
+      <c r="O114">
+        <v>83</v>
+      </c>
+      <c r="P114">
+        <v>14</v>
+      </c>
+      <c r="Q114">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A115" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B115" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C115" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D115" s="11">
+        <v>13</v>
+      </c>
+      <c r="E115" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G115" t="s">
+        <v>37</v>
+      </c>
+      <c r="H115" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I115" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="K115" t="s">
+        <v>119</v>
+      </c>
+      <c r="L115">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="O115">
+        <v>188</v>
+      </c>
+      <c r="P115">
+        <v>14</v>
+      </c>
+      <c r="Q115">
+        <f t="shared" si="0"/>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A116" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B116" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C116" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D116" s="11">
+        <v>14</v>
+      </c>
+      <c r="E116" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G116" t="s">
+        <v>26</v>
+      </c>
+      <c r="H116" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I116" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="M116">
+        <v>98</v>
+      </c>
+      <c r="N116">
+        <v>60</v>
+      </c>
+      <c r="O116">
+        <v>180</v>
+      </c>
+      <c r="P116">
+        <v>14</v>
+      </c>
+      <c r="Q116">
+        <f t="shared" si="0"/>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="117" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A117" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B117" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C117" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D117" s="11">
+        <v>15</v>
+      </c>
+      <c r="E117" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H117" s="15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A118" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B118" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C118" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D118" s="11">
+        <v>16</v>
+      </c>
+      <c r="E118" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G118" t="s">
+        <v>26</v>
+      </c>
+      <c r="H118" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I118" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="M118">
+        <v>92</v>
+      </c>
+      <c r="N118">
+        <v>48</v>
+      </c>
+      <c r="O118">
+        <v>166</v>
+      </c>
+      <c r="P118">
+        <v>14</v>
+      </c>
+      <c r="Q118">
+        <f t="shared" si="0"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="119" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A119" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B119" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C119" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D119" s="11">
+        <v>17</v>
+      </c>
+      <c r="E119" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G119" t="s">
+        <v>26</v>
+      </c>
+      <c r="H119" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I119" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="M119">
+        <v>93</v>
+      </c>
+      <c r="N119">
+        <v>46</v>
+      </c>
+      <c r="O119">
+        <v>150</v>
+      </c>
+      <c r="P119">
+        <v>14</v>
+      </c>
+      <c r="Q119">
+        <f>O119-P119</f>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="120" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A120" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B120" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C120" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D120" s="11">
+        <v>18</v>
+      </c>
+      <c r="E120" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H120" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I120" s="15"/>
+      <c r="U120" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A121" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B121" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C121" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D121" s="11">
+        <v>19</v>
+      </c>
+      <c r="E121" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H121" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I121" s="15"/>
+      <c r="U121" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="122" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A122" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B122" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C122" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D122" s="11">
+        <v>20</v>
+      </c>
+      <c r="E122" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G122" t="s">
+        <v>26</v>
+      </c>
+      <c r="H122" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I122" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="M122">
+        <v>114</v>
+      </c>
+      <c r="N122">
+        <v>60</v>
+      </c>
+      <c r="O122">
+        <v>178</v>
+      </c>
+      <c r="P122">
+        <v>14</v>
+      </c>
+      <c r="Q122">
+        <f>O122-P122</f>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="123" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A123" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B123" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C123" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D123" s="11">
+        <v>21</v>
+      </c>
+      <c r="E123" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G123" t="s">
+        <v>37</v>
+      </c>
+      <c r="H123" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I123" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="K123" t="s">
+        <v>113</v>
+      </c>
+      <c r="L123">
+        <v>10.7</v>
+      </c>
+      <c r="O123">
+        <v>174</v>
+      </c>
+      <c r="P123">
+        <v>14</v>
+      </c>
+      <c r="Q123">
+        <f>O123-P123</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="124" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A124" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B124" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C124" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D124" s="11">
+        <v>22</v>
+      </c>
+      <c r="E124" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G124" t="s">
+        <v>37</v>
+      </c>
+      <c r="H124" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I124" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="K124" t="s">
+        <v>113</v>
+      </c>
+      <c r="L124">
+        <v>909</v>
+      </c>
+      <c r="O124">
+        <v>175</v>
+      </c>
+      <c r="P124">
+        <v>14</v>
+      </c>
+      <c r="Q124">
+        <f t="shared" si="0"/>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="125" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A125" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B125" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C125" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D125" s="11">
+        <v>23</v>
+      </c>
+      <c r="E125" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G125" t="s">
+        <v>26</v>
+      </c>
+      <c r="H125" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I125" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="M125">
+        <v>98</v>
+      </c>
+      <c r="N125">
+        <v>55</v>
+      </c>
+      <c r="O125">
+        <v>158</v>
+      </c>
+      <c r="P125">
+        <v>14</v>
+      </c>
+      <c r="Q125">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="126" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A126" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B126" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C126" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D126" s="11">
+        <v>24</v>
+      </c>
+      <c r="E126" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H126" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I126" s="15"/>
+    </row>
+    <row r="127" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A127" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B127" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C127" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D127" s="17">
+        <v>25</v>
+      </c>
+      <c r="E127" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G127" t="s">
+        <v>26</v>
+      </c>
+      <c r="H127" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I127" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="M127">
+        <v>81</v>
+      </c>
+      <c r="N127">
+        <v>48</v>
+      </c>
+      <c r="O127">
+        <v>132</v>
+      </c>
+      <c r="P127">
+        <v>14</v>
+      </c>
+      <c r="Q127">
+        <f t="shared" si="0"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="128" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A128" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B128" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C128" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D128" s="11">
+        <v>26</v>
+      </c>
+      <c r="E128" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G128" t="s">
+        <v>26</v>
+      </c>
+      <c r="H128" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I128" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="M128">
+        <v>94</v>
+      </c>
+      <c r="N128">
+        <v>40</v>
+      </c>
+      <c r="O128">
+        <v>142</v>
+      </c>
+      <c r="P128">
+        <v>14</v>
+      </c>
+      <c r="Q128">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="129" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A129" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B129" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C129" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D129" s="11">
+        <v>27</v>
+      </c>
+      <c r="E129" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G129" t="s">
+        <v>26</v>
+      </c>
+      <c r="H129" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I129" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="M129">
+        <v>95</v>
+      </c>
+      <c r="N129">
+        <v>56</v>
+      </c>
+      <c r="O129">
+        <v>160</v>
+      </c>
+      <c r="P129">
+        <v>14</v>
+      </c>
+      <c r="Q129">
+        <f t="shared" si="0"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="130" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A130" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B130" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C130" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D130" s="17">
+        <v>28</v>
+      </c>
+      <c r="E130" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G130" t="s">
+        <v>26</v>
+      </c>
+      <c r="H130" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I130" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="M130">
+        <v>97</v>
+      </c>
+      <c r="N130">
+        <v>44</v>
+      </c>
+      <c r="O130">
+        <v>155</v>
+      </c>
+      <c r="P130">
+        <v>14</v>
+      </c>
+      <c r="Q130">
+        <f t="shared" si="0"/>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="131" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A131" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B131" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C131" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D131" s="11">
+        <v>29</v>
+      </c>
+      <c r="E131" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G131" t="s">
+        <v>37</v>
+      </c>
+      <c r="H131" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I131" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="K131" t="s">
+        <v>117</v>
+      </c>
+      <c r="L131">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="O131">
+        <v>164</v>
+      </c>
+      <c r="P131">
+        <v>14</v>
+      </c>
+      <c r="Q131">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="132" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A132" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B132" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C132" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D132" s="11">
+        <v>30</v>
+      </c>
+      <c r="E132" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G132" t="s">
+        <v>26</v>
+      </c>
+      <c r="H132" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="I132" s="15"/>
+      <c r="M132">
+        <v>54</v>
+      </c>
+      <c r="N132">
+        <v>19</v>
+      </c>
+      <c r="O132">
+        <v>108</v>
+      </c>
+      <c r="P132">
+        <v>14</v>
+      </c>
+      <c r="Q132">
+        <f t="shared" si="0"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="133" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A133" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B133" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C133" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D133" s="17">
+        <v>31</v>
+      </c>
+      <c r="E133" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G133" t="s">
+        <v>26</v>
+      </c>
+      <c r="H133" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I133" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="M133">
+        <v>97</v>
+      </c>
+      <c r="N133">
+        <v>51</v>
+      </c>
+      <c r="O133">
+        <v>158</v>
+      </c>
+      <c r="P133">
+        <v>14</v>
+      </c>
+      <c r="Q133">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="134" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A134" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B134" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C134" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D134" s="17">
+        <v>32</v>
+      </c>
+      <c r="E134" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G134" t="s">
+        <v>26</v>
+      </c>
+      <c r="H134" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I134" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="M134">
+        <v>13</v>
+      </c>
+      <c r="N134">
+        <v>59</v>
+      </c>
+      <c r="O134">
+        <v>164</v>
+      </c>
+      <c r="P134">
+        <v>14</v>
+      </c>
+      <c r="Q134">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="135" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A135" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B135" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C135" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D135" s="11">
+        <v>33</v>
+      </c>
+      <c r="E135" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G135" t="s">
+        <v>37</v>
+      </c>
+      <c r="H135" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I135" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="K135" t="s">
+        <v>119</v>
+      </c>
+      <c r="L135">
+        <v>9.5</v>
+      </c>
+      <c r="O135">
+        <v>174</v>
+      </c>
+      <c r="P135">
+        <v>14</v>
+      </c>
+      <c r="Q135">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="136" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A136" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B136" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C136" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D136" s="11">
+        <v>34</v>
+      </c>
+      <c r="E136" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G136" t="s">
+        <v>26</v>
+      </c>
+      <c r="H136" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I136" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="M136">
+        <v>95</v>
+      </c>
+      <c r="N136">
+        <v>46</v>
+      </c>
+      <c r="O136">
+        <v>142</v>
+      </c>
+      <c r="P136">
+        <v>14</v>
+      </c>
+      <c r="Q136">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="137" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A137" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B137" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C137" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D137" s="11">
+        <v>35</v>
+      </c>
+      <c r="E137" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H137" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I137" s="15"/>
+      <c r="U137" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="138" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A138" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B138" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C138" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D138" s="11">
+        <v>36</v>
+      </c>
+      <c r="E138" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H138" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I138" s="15"/>
+      <c r="U138" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="139" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A139" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B139" s="39">
+        <v>2016</v>
+      </c>
+      <c r="C139" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="D139" s="40">
+        <v>37</v>
+      </c>
+      <c r="E139" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H139" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="140" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A140" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B140" s="39">
+        <v>2016</v>
+      </c>
+      <c r="C140" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="D140" s="40">
+        <v>38</v>
+      </c>
+      <c r="E140" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G140" t="s">
+        <v>26</v>
+      </c>
+      <c r="H140" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I140" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="M140">
+        <v>96</v>
+      </c>
+      <c r="N140">
+        <v>51</v>
+      </c>
+      <c r="O140">
+        <v>164</v>
+      </c>
+      <c r="P140">
+        <v>14</v>
+      </c>
+      <c r="Q140">
+        <f>O140-P140</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="141" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A141" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B141" s="39">
+        <v>2016</v>
+      </c>
+      <c r="C141" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="D141" s="40">
+        <v>39</v>
+      </c>
+      <c r="E141" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G141" t="s">
+        <v>37</v>
+      </c>
+      <c r="H141" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I141" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="K141" t="s">
+        <v>113</v>
+      </c>
+      <c r="L141">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="O141">
+        <v>186</v>
+      </c>
+      <c r="P141">
+        <v>14</v>
+      </c>
+      <c r="Q141">
+        <f t="shared" si="0"/>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="142" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A142" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B142" s="39">
+        <v>2016</v>
+      </c>
+      <c r="C142" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="D142" s="40">
+        <v>40</v>
+      </c>
+      <c r="E142" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G142" t="s">
+        <v>26</v>
+      </c>
+      <c r="H142" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I142" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="M142">
+        <v>76</v>
+      </c>
+      <c r="N142">
+        <v>35</v>
+      </c>
+      <c r="O142">
+        <v>145</v>
+      </c>
+      <c r="P142">
+        <v>14</v>
+      </c>
+      <c r="Q142">
+        <f t="shared" si="0"/>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="143" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A143" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B143" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C143" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D143" s="17">
+        <v>41</v>
+      </c>
+      <c r="E143" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G143" t="s">
+        <v>37</v>
+      </c>
+      <c r="H143" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I143" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="K143" t="s">
+        <v>113</v>
+      </c>
+      <c r="L143">
+        <v>9.5</v>
+      </c>
+      <c r="O143">
+        <v>172</v>
+      </c>
+      <c r="P143">
+        <v>14</v>
+      </c>
+      <c r="Q143">
+        <f t="shared" si="0"/>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="144" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A144" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B144" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C144" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D144" s="11">
+        <v>42</v>
+      </c>
+      <c r="E144" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G144" t="s">
+        <v>26</v>
+      </c>
+      <c r="H144" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I144" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="M144">
+        <v>76</v>
+      </c>
+      <c r="N144">
+        <v>38</v>
+      </c>
+      <c r="O144">
+        <v>140</v>
+      </c>
+      <c r="P144">
+        <v>14</v>
+      </c>
+      <c r="Q144">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="145" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A145" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B145" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C145" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D145" s="11">
+        <v>43</v>
+      </c>
+      <c r="E145" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G145" t="s">
+        <v>37</v>
+      </c>
+      <c r="H145" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I145" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="K145" t="s">
+        <v>113</v>
+      </c>
+      <c r="L145">
+        <v>10.8</v>
+      </c>
+      <c r="O145">
+        <v>200</v>
+      </c>
+      <c r="P145">
+        <v>14</v>
+      </c>
+      <c r="Q145">
+        <f t="shared" si="0"/>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="146" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A146" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B146" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C146" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D146" s="11">
+        <v>45</v>
+      </c>
+      <c r="E146" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G146" t="s">
+        <v>37</v>
+      </c>
+      <c r="H146" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I146" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="K146" t="s">
+        <v>113</v>
+      </c>
+      <c r="L146">
+        <v>7.9</v>
+      </c>
+      <c r="O146">
+        <v>168</v>
+      </c>
+      <c r="P146">
+        <v>14</v>
+      </c>
+      <c r="Q146">
+        <f t="shared" si="0"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="147" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A147" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B147" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C147" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D147" s="11">
+        <v>46</v>
+      </c>
+      <c r="E147" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H147" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I147" s="15"/>
+    </row>
+    <row r="148" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A148" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B148" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C148" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D148" s="11">
+        <v>47</v>
+      </c>
+      <c r="E148" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G148" t="s">
+        <v>37</v>
+      </c>
+      <c r="H148" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I148" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="K148" t="s">
+        <v>113</v>
+      </c>
+      <c r="L148" t="s">
+        <v>147</v>
+      </c>
+      <c r="O148">
+        <v>198</v>
+      </c>
+      <c r="P148">
+        <v>14</v>
+      </c>
+      <c r="Q148">
+        <f t="shared" si="0"/>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="149" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A149" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B149" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C149" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D149" s="11">
+        <v>48</v>
+      </c>
+      <c r="E149" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H149" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I149" s="15"/>
+    </row>
+    <row r="150" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A150" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B150" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C150" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D150" s="11">
+        <v>1</v>
+      </c>
+      <c r="E150" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G150" t="s">
+        <v>37</v>
+      </c>
+      <c r="H150" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I150" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="K150" t="s">
+        <v>113</v>
+      </c>
+      <c r="L150">
+        <v>10.7</v>
+      </c>
+      <c r="O150">
+        <v>178</v>
+      </c>
+      <c r="P150">
+        <v>14</v>
+      </c>
+      <c r="Q150">
+        <f>O150-P150</f>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="151" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A151" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B151" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C151" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D151" s="11">
+        <v>2</v>
+      </c>
+      <c r="E151" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="H151" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I151" s="15"/>
+    </row>
+    <row r="152" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A152" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B152" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C152" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D152" s="11">
+        <v>3</v>
+      </c>
+      <c r="E152" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G152" t="s">
+        <v>26</v>
+      </c>
+      <c r="H152" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I152" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="M152">
+        <v>96</v>
+      </c>
+      <c r="N152">
+        <v>46</v>
+      </c>
+      <c r="O152">
+        <v>158</v>
+      </c>
+      <c r="P152">
+        <v>14</v>
+      </c>
+      <c r="Q152">
+        <f t="shared" ref="Q152:Q169" si="1">O152-P152</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="153" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A153" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B153" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C153" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D153" s="17">
+        <v>4</v>
+      </c>
+      <c r="E153" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G153" t="s">
+        <v>37</v>
+      </c>
+      <c r="H153" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I153" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="K153">
+        <v>11</v>
+      </c>
+      <c r="L153" t="s">
+        <v>147</v>
+      </c>
+      <c r="O153" t="s">
+        <v>147</v>
+      </c>
+      <c r="U153" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="154" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A154" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B154" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C154" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D154" s="11">
+        <v>5</v>
+      </c>
+      <c r="E154" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G154" t="s">
+        <v>37</v>
+      </c>
+      <c r="H154" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I154" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="K154" t="s">
+        <v>119</v>
+      </c>
+      <c r="L154">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="O154">
+        <v>184</v>
+      </c>
+      <c r="P154">
+        <v>14</v>
+      </c>
+      <c r="Q154">
+        <f t="shared" si="1"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="155" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A155" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B155" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C155" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D155" s="11">
+        <v>6</v>
+      </c>
+      <c r="E155" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G155" t="s">
+        <v>37</v>
+      </c>
+      <c r="H155" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I155" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="K155" t="s">
+        <v>113</v>
+      </c>
+      <c r="L155">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="O155">
+        <v>192</v>
+      </c>
+      <c r="P155">
+        <v>14</v>
+      </c>
+      <c r="Q155">
+        <f t="shared" si="1"/>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="156" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A156" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B156" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C156" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D156" s="11">
+        <v>7</v>
+      </c>
+      <c r="E156" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G156" t="s">
+        <v>26</v>
+      </c>
+      <c r="H156" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="I156" s="15"/>
+      <c r="M156">
+        <v>35</v>
+      </c>
+      <c r="N156">
+        <v>5</v>
+      </c>
+      <c r="O156">
+        <v>83</v>
+      </c>
+      <c r="P156">
+        <v>14</v>
+      </c>
+      <c r="Q156">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="U156" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="157" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A157" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B157" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C157" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D157" s="11">
+        <v>8</v>
+      </c>
+      <c r="E157" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G157" t="s">
+        <v>26</v>
+      </c>
+      <c r="H157" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I157" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="M157">
+        <v>98</v>
+      </c>
+      <c r="N157">
+        <v>50</v>
+      </c>
+      <c r="O157">
+        <v>140</v>
+      </c>
+      <c r="P157">
+        <v>14</v>
+      </c>
+      <c r="Q157">
+        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="158" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A158" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B158" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C158" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D158" s="11">
+        <v>9</v>
+      </c>
+      <c r="E158" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G158" t="s">
+        <v>26</v>
+      </c>
+      <c r="H158" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I158" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="M158">
+        <v>90</v>
+      </c>
+      <c r="N158">
+        <v>36</v>
+      </c>
+      <c r="O158">
+        <v>140</v>
+      </c>
+      <c r="P158">
+        <v>14</v>
+      </c>
+      <c r="Q158">
+        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="159" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A159" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B159" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C159" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D159" s="11">
+        <v>10</v>
+      </c>
+      <c r="E159" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="H159" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I159" s="15"/>
+    </row>
+    <row r="160" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A160" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B160" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C160" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D160" s="11">
+        <v>11</v>
+      </c>
+      <c r="E160" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G160" t="s">
+        <v>37</v>
+      </c>
+      <c r="H160" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I160" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="K160" t="s">
+        <v>113</v>
+      </c>
+      <c r="L160">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="O160">
+        <v>200</v>
+      </c>
+      <c r="P160">
+        <v>14</v>
+      </c>
+      <c r="Q160">
+        <f t="shared" si="1"/>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="161" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A161" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B161" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C161" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D161" s="11">
+        <v>12</v>
+      </c>
+      <c r="E161" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G161" t="s">
+        <v>26</v>
+      </c>
+      <c r="H161" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I161" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="M161">
+        <v>114</v>
+      </c>
+      <c r="N161">
+        <v>68</v>
+      </c>
+      <c r="O161">
+        <v>142</v>
+      </c>
+      <c r="P161">
+        <v>14</v>
+      </c>
+      <c r="Q161">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="162" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A162" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B162" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C162" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D162" s="17">
+        <v>13</v>
+      </c>
+      <c r="E162" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G162" t="s">
+        <v>26</v>
+      </c>
+      <c r="H162" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I162" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="M162">
+        <v>101</v>
+      </c>
+      <c r="N162">
+        <v>56</v>
+      </c>
+      <c r="O162">
+        <v>176</v>
+      </c>
+      <c r="P162">
+        <v>14</v>
+      </c>
+      <c r="Q162">
+        <f t="shared" si="1"/>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="163" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A163" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B163" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C163" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D163" s="11">
+        <v>14</v>
+      </c>
+      <c r="E163" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G163" t="s">
+        <v>26</v>
+      </c>
+      <c r="H163" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I163" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="M163">
+        <v>105</v>
+      </c>
+      <c r="N163">
+        <v>55</v>
+      </c>
+      <c r="O163">
+        <v>150</v>
+      </c>
+      <c r="P163">
+        <v>14</v>
+      </c>
+      <c r="Q163">
+        <f t="shared" si="1"/>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="164" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A164" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B164" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C164" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D164" s="17">
+        <v>15</v>
+      </c>
+      <c r="E164" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="H164" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I164" s="15"/>
+    </row>
+    <row r="165" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A165" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B165" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C165" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D165" s="17">
+        <v>16</v>
+      </c>
+      <c r="E165" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G165" t="s">
+        <v>26</v>
+      </c>
+      <c r="H165" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I165" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="M165">
+        <v>103</v>
+      </c>
+      <c r="N165">
+        <v>51</v>
+      </c>
+      <c r="O165">
+        <v>160</v>
+      </c>
+      <c r="P165">
+        <v>14</v>
+      </c>
+      <c r="Q165">
+        <f t="shared" si="1"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="166" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A166" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B166" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C166" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D166" s="17">
+        <v>17</v>
+      </c>
+      <c r="E166" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G166" t="s">
+        <v>37</v>
+      </c>
+      <c r="H166" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I166" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="K166" t="s">
+        <v>119</v>
+      </c>
+      <c r="L166">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="O166">
+        <v>196</v>
+      </c>
+      <c r="P166">
+        <v>14</v>
+      </c>
+      <c r="Q166">
+        <f t="shared" si="1"/>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="167" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A167" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B167" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C167" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D167" s="11">
+        <v>18</v>
+      </c>
+      <c r="E167" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="H167" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="I167" s="15"/>
+      <c r="U167" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="168" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A168" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B168" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C168" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D168" s="11">
+        <v>19</v>
+      </c>
+      <c r="E168" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G168" t="s">
+        <v>26</v>
+      </c>
+      <c r="H168" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="I168" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="M168">
+        <v>79</v>
+      </c>
+      <c r="N168">
+        <v>36</v>
+      </c>
+      <c r="O168">
+        <v>134</v>
+      </c>
+      <c r="P168">
+        <v>14</v>
+      </c>
+      <c r="Q168">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="169" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A169" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B169" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C169" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D169" s="17">
+        <v>20</v>
+      </c>
+      <c r="E169" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G169" t="s">
+        <v>26</v>
+      </c>
+      <c r="H169" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I169" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="M169">
+        <v>101</v>
+      </c>
+      <c r="N169">
+        <v>53</v>
+      </c>
+      <c r="O169">
+        <v>154</v>
+      </c>
+      <c r="P169">
+        <v>14</v>
+      </c>
+      <c r="Q169">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="170" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A170" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B170" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C170" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D170" s="11">
+        <v>21</v>
+      </c>
+      <c r="E170" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="H170" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I170" s="15"/>
+    </row>
+    <row r="171" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A171" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B171" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C171" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D171" s="11">
+        <v>22</v>
+      </c>
+      <c r="E171" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="H171" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I171" s="15"/>
+    </row>
+    <row r="172" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A172" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B172" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C172" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D172" s="11">
+        <v>23</v>
+      </c>
+      <c r="E172" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G172" t="s">
+        <v>26</v>
+      </c>
+      <c r="H172" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I172" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="M172">
+        <v>108</v>
+      </c>
+      <c r="N172">
+        <v>61</v>
+      </c>
+      <c r="O172">
+        <v>158</v>
+      </c>
+      <c r="P172">
+        <v>14</v>
+      </c>
+      <c r="Q172">
+        <f>O172-P172</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="173" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A173" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B173" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C173" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D173" s="11">
+        <v>24</v>
+      </c>
+      <c r="E173" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G173" t="s">
+        <v>37</v>
+      </c>
+      <c r="H173" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I173" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="K173" t="s">
+        <v>117</v>
+      </c>
+      <c r="L173">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="O173">
+        <v>172</v>
+      </c>
+      <c r="P173">
+        <v>14</v>
+      </c>
+      <c r="Q173">
+        <f>O173-P173</f>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="174" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A174" s="37">
+        <v>42463</v>
+      </c>
+      <c r="B174" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C174" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D174" s="11">
+        <v>25</v>
+      </c>
+      <c r="E174" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="H174" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I174" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4930,9 +7726,9 @@
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="27"/>
       <c r="B1" s="28"/>
       <c r="C1" s="29"/>
@@ -4947,7 +7743,7 @@
       <c r="J1" s="29"/>
       <c r="K1" s="29"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>70</v>
       </c>
@@ -4970,7 +7766,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>75</v>
       </c>
@@ -4989,7 +7785,7 @@
       <c r="J3" s="30"/>
       <c r="K3" s="30"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
         <v>78</v>
       </c>
@@ -5008,7 +7804,7 @@
       <c r="J4" s="31"/>
       <c r="K4" s="31"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
         <v>81</v>
       </c>
@@ -5027,7 +7823,7 @@
       <c r="J5" s="30"/>
       <c r="K5" s="30"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>84</v>
       </c>
@@ -5046,7 +7842,7 @@
       <c r="J6" s="30"/>
       <c r="K6" s="30"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="27"/>
       <c r="B7" s="28"/>
       <c r="C7" s="29"/>
@@ -5061,7 +7857,7 @@
       <c r="J7" s="30"/>
       <c r="K7" s="30"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="27"/>
       <c r="B8" s="28"/>
       <c r="C8" s="29"/>
@@ -5076,7 +7872,7 @@
       <c r="J8" s="30"/>
       <c r="K8" s="30"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="27"/>
       <c r="B9" s="28"/>
       <c r="C9" s="29"/>
@@ -5091,7 +7887,7 @@
       <c r="J9" s="30"/>
       <c r="K9" s="30"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="27"/>
       <c r="B10" s="28"/>
       <c r="C10" s="29"/>
@@ -5106,7 +7902,7 @@
       <c r="J10" s="30"/>
       <c r="K10" s="30"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="27"/>
       <c r="B11" s="28"/>
       <c r="C11" s="29"/>
@@ -5119,7 +7915,7 @@
       <c r="J11" s="29"/>
       <c r="K11" s="29"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
         <v>91</v>
       </c>
@@ -5133,7 +7929,7 @@
       <c r="I13" s="32"/>
       <c r="J13" s="32"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="33"/>
       <c r="B14" s="34"/>
       <c r="C14" s="34"/>
@@ -5149,7 +7945,7 @@
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
         <v>70</v>
       </c>
@@ -5169,7 +7965,7 @@
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
         <v>75</v>
       </c>
@@ -5189,7 +7985,7 @@
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
         <v>78</v>
       </c>
@@ -5209,7 +8005,7 @@
       <c r="I17" s="32"/>
       <c r="J17" s="32"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
         <v>81</v>
       </c>
@@ -5229,7 +8025,7 @@
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
         <v>84</v>
       </c>
@@ -5249,7 +8045,7 @@
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="33"/>
       <c r="B20" s="34"/>
       <c r="C20" s="34"/>
@@ -5265,7 +8061,7 @@
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="33"/>
       <c r="B21" s="34"/>
       <c r="C21" s="34"/>
@@ -5281,7 +8077,7 @@
       <c r="I21" s="32"/>
       <c r="J21" s="32"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="33"/>
       <c r="B22" s="34"/>
       <c r="C22" s="34"/>
@@ -5297,7 +8093,7 @@
       <c r="I22" s="32"/>
       <c r="J22" s="32"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="33"/>
       <c r="B23" s="34"/>
       <c r="C23" s="34"/>
@@ -5313,7 +8109,7 @@
       <c r="I23" s="32"/>
       <c r="J23" s="32"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="33"/>
       <c r="B24" s="34"/>
       <c r="C24" s="34"/>
@@ -5329,7 +8125,7 @@
       <c r="I24" s="32"/>
       <c r="J24" s="32"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="33"/>
       <c r="B25" s="34"/>
       <c r="C25" s="34"/>
@@ -5345,7 +8141,7 @@
       <c r="I25" s="32"/>
       <c r="J25" s="32"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="32"/>
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>

</xml_diff>

<commit_message>
proofed May CAAU box check data
</commit_message>
<xml_diff>
--- a/caau_monitoring_2016_PI_shared.xlsx
+++ b/caau_monitoring_2016_PI_shared.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="166">
   <si>
     <t>Date</t>
   </si>
@@ -345,9 +345,6 @@
     <t>AD = ADULT</t>
   </si>
   <si>
-    <t>EMPTRY</t>
-  </si>
-  <si>
     <t>ALMOST DEAD, COVERED IN LITTLE RED BUGS, DIDN'T PROCESS</t>
   </si>
   <si>
@@ -514,9 +511,6 @@
   </si>
   <si>
     <t>NEWLY-HATCHED CHICK SIZED, PRETTY FRESH</t>
-  </si>
-  <si>
-    <t>LCG</t>
   </si>
   <si>
     <t>1643-03623</t>
@@ -1005,7 +999,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A141" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R174" sqref="R174"/>
+      <selection pane="bottomLeft" activeCell="G174" sqref="G174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5131,7 +5125,7 @@
         <v>22</v>
       </c>
       <c r="H103" s="15" t="s">
-        <v>106</v>
+        <v>23</v>
       </c>
       <c r="Q103" s="12">
         <f>O103-P103</f>
@@ -5161,7 +5155,7 @@
         <v>28</v>
       </c>
       <c r="U104" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="105" spans="1:25" x14ac:dyDescent="0.25">
@@ -5187,7 +5181,7 @@
         <v>28</v>
       </c>
       <c r="I105" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M105">
         <v>96</v>
@@ -5226,7 +5220,7 @@
         <v>23</v>
       </c>
       <c r="U106" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="107" spans="1:25" x14ac:dyDescent="0.25">
@@ -5272,7 +5266,7 @@
         <v>31</v>
       </c>
       <c r="I108" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M108">
         <v>104</v>
@@ -5334,7 +5328,7 @@
         <v>31</v>
       </c>
       <c r="I110" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M110">
         <v>101</v>
@@ -5376,10 +5370,10 @@
         <v>38</v>
       </c>
       <c r="I111" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="K111" t="s">
         <v>112</v>
-      </c>
-      <c r="K111" t="s">
-        <v>113</v>
       </c>
       <c r="L111">
         <v>9.1999999999999993</v>
@@ -5418,10 +5412,10 @@
         <v>38</v>
       </c>
       <c r="I112" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K112" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L112">
         <v>9.3000000000000007</v>
@@ -5437,7 +5431,7 @@
         <v>174</v>
       </c>
       <c r="U112" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="113" spans="1:21" x14ac:dyDescent="0.25">
@@ -5463,10 +5457,10 @@
         <v>38</v>
       </c>
       <c r="I113" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="K113" t="s">
         <v>116</v>
-      </c>
-      <c r="K113" t="s">
-        <v>117</v>
       </c>
       <c r="L113">
         <v>9.1999999999999993</v>
@@ -5544,10 +5538,10 @@
         <v>38</v>
       </c>
       <c r="I115" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="K115" t="s">
         <v>118</v>
-      </c>
-      <c r="K115" t="s">
-        <v>119</v>
       </c>
       <c r="L115">
         <v>9.3000000000000007</v>
@@ -5586,7 +5580,7 @@
         <v>31</v>
       </c>
       <c r="I116" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M116">
         <v>98</v>
@@ -5621,8 +5615,11 @@
       <c r="E117" s="14" t="s">
         <v>22</v>
       </c>
+      <c r="G117" s="15" t="s">
+        <v>120</v>
+      </c>
       <c r="H117" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="118" spans="1:21" x14ac:dyDescent="0.25">
@@ -5648,7 +5645,7 @@
         <v>28</v>
       </c>
       <c r="I118" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M118">
         <v>92</v>
@@ -5690,7 +5687,7 @@
         <v>28</v>
       </c>
       <c r="I119" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M119">
         <v>93</v>
@@ -5730,7 +5727,7 @@
       </c>
       <c r="I120" s="15"/>
       <c r="U120" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="121" spans="1:21" x14ac:dyDescent="0.25">
@@ -5754,7 +5751,7 @@
       </c>
       <c r="I121" s="15"/>
       <c r="U121" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="122" spans="1:21" x14ac:dyDescent="0.25">
@@ -5780,7 +5777,7 @@
         <v>31</v>
       </c>
       <c r="I122" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M122">
         <v>114</v>
@@ -5822,10 +5819,10 @@
         <v>55</v>
       </c>
       <c r="I123" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K123" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L123">
         <v>10.7</v>
@@ -5864,13 +5861,13 @@
         <v>38</v>
       </c>
       <c r="I124" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K124" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L124">
-        <v>909</v>
+        <v>9.9</v>
       </c>
       <c r="O124">
         <v>175</v>
@@ -5906,7 +5903,7 @@
         <v>31</v>
       </c>
       <c r="I125" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M125">
         <v>98</v>
@@ -5969,7 +5966,7 @@
         <v>57</v>
       </c>
       <c r="I127" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M127">
         <v>81</v>
@@ -6011,7 +6008,7 @@
         <v>28</v>
       </c>
       <c r="I128" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M128">
         <v>94</v>
@@ -6053,7 +6050,7 @@
         <v>28</v>
       </c>
       <c r="I129" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M129">
         <v>95</v>
@@ -6095,7 +6092,7 @@
         <v>28</v>
       </c>
       <c r="I130" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M130">
         <v>97</v>
@@ -6137,10 +6134,10 @@
         <v>38</v>
       </c>
       <c r="I131" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K131" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L131">
         <v>8.8000000000000007</v>
@@ -6219,7 +6216,7 @@
         <v>28</v>
       </c>
       <c r="I133" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M133">
         <v>97</v>
@@ -6261,10 +6258,10 @@
         <v>28</v>
       </c>
       <c r="I134" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M134">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="N134">
         <v>59</v>
@@ -6303,10 +6300,10 @@
         <v>38</v>
       </c>
       <c r="I135" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K135" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L135">
         <v>9.5</v>
@@ -6345,7 +6342,7 @@
         <v>28</v>
       </c>
       <c r="I136" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M136">
         <v>95</v>
@@ -6385,7 +6382,7 @@
       </c>
       <c r="I137" s="15"/>
       <c r="U137" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="138" spans="1:21" x14ac:dyDescent="0.25">
@@ -6409,7 +6406,7 @@
       </c>
       <c r="I138" s="15"/>
       <c r="U138" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="139" spans="1:21" x14ac:dyDescent="0.25">
@@ -6455,7 +6452,7 @@
         <v>31</v>
       </c>
       <c r="I140" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M140">
         <v>96</v>
@@ -6497,10 +6494,10 @@
         <v>38</v>
       </c>
       <c r="I141" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K141" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L141">
         <v>9.8000000000000007</v>
@@ -6539,7 +6536,7 @@
         <v>28</v>
       </c>
       <c r="I142" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M142">
         <v>76</v>
@@ -6581,10 +6578,10 @@
         <v>55</v>
       </c>
       <c r="I143" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K143" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L143">
         <v>9.5</v>
@@ -6623,7 +6620,7 @@
         <v>57</v>
       </c>
       <c r="I144" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M144">
         <v>76</v>
@@ -6665,10 +6662,10 @@
         <v>38</v>
       </c>
       <c r="I145" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K145" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L145">
         <v>10.8</v>
@@ -6707,10 +6704,10 @@
         <v>38</v>
       </c>
       <c r="I146" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K146" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L146">
         <v>7.9</v>
@@ -6770,13 +6767,13 @@
         <v>38</v>
       </c>
       <c r="I148" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="K148" t="s">
+        <v>112</v>
+      </c>
+      <c r="L148" t="s">
         <v>146</v>
-      </c>
-      <c r="K148" t="s">
-        <v>113</v>
-      </c>
-      <c r="L148" t="s">
-        <v>147</v>
       </c>
       <c r="O148">
         <v>198</v>
@@ -6833,10 +6830,10 @@
         <v>38</v>
       </c>
       <c r="I150" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K150" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L150">
         <v>10.7</v>
@@ -6896,7 +6893,7 @@
         <v>28</v>
       </c>
       <c r="I152" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M152">
         <v>96</v>
@@ -6940,17 +6937,17 @@
       <c r="I153" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="K153">
-        <v>11</v>
+      <c r="K153" t="s">
+        <v>118</v>
       </c>
       <c r="L153" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O153" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="U153" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="154" spans="1:21" x14ac:dyDescent="0.25">
@@ -6976,10 +6973,10 @@
         <v>38</v>
       </c>
       <c r="I154" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K154" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L154">
         <v>9.3000000000000007</v>
@@ -7018,10 +7015,10 @@
         <v>38</v>
       </c>
       <c r="I155" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K155" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L155">
         <v>8.6999999999999993</v>
@@ -7077,7 +7074,7 @@
         <v>69</v>
       </c>
       <c r="U156" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="157" spans="1:21" x14ac:dyDescent="0.25">
@@ -7103,7 +7100,7 @@
         <v>28</v>
       </c>
       <c r="I157" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M157">
         <v>98</v>
@@ -7145,7 +7142,7 @@
         <v>28</v>
       </c>
       <c r="I158" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M158">
         <v>90</v>
@@ -7208,10 +7205,10 @@
         <v>38</v>
       </c>
       <c r="I160" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K160" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L160">
         <v>10.199999999999999</v>
@@ -7250,7 +7247,7 @@
         <v>31</v>
       </c>
       <c r="I161" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M161">
         <v>114</v>
@@ -7292,7 +7289,7 @@
         <v>28</v>
       </c>
       <c r="I162" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M162">
         <v>101</v>
@@ -7334,7 +7331,7 @@
         <v>28</v>
       </c>
       <c r="I163" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M163">
         <v>105</v>
@@ -7397,7 +7394,7 @@
         <v>28</v>
       </c>
       <c r="I165" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M165">
         <v>103</v>
@@ -7439,10 +7436,10 @@
         <v>38</v>
       </c>
       <c r="I166" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K166" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L166">
         <v>9.8000000000000007</v>
@@ -7479,7 +7476,7 @@
       </c>
       <c r="I167" s="15"/>
       <c r="U167" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="168" spans="1:21" x14ac:dyDescent="0.25">
@@ -7502,10 +7499,10 @@
         <v>26</v>
       </c>
       <c r="H168" s="15" t="s">
-        <v>163</v>
+        <v>57</v>
       </c>
       <c r="I168" s="15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="M168">
         <v>79</v>
@@ -7547,7 +7544,7 @@
         <v>28</v>
       </c>
       <c r="I169" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="M169">
         <v>101</v>
@@ -7631,7 +7628,7 @@
         <v>31</v>
       </c>
       <c r="I172" s="15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="M172">
         <v>108</v>
@@ -7673,10 +7670,10 @@
         <v>38</v>
       </c>
       <c r="I173" s="15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K173" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L173">
         <v>8.6999999999999993</v>

</xml_diff>

<commit_message>
Data entry PI 6/2016
CAAU, ASSP+CAAU BBL
</commit_message>
<xml_diff>
--- a/caau_monitoring_2016_PI_shared.xlsx
+++ b/caau_monitoring_2016_PI_shared.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekelsey\Documents\WERC-SC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mczapanskiy\Documents\GitHub\WERC-SC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="222">
   <si>
     <t>Date</t>
   </si>
@@ -523,6 +523,174 @@
   </si>
   <si>
     <t>1643-10414</t>
+  </si>
+  <si>
+    <t>1643-03655</t>
+  </si>
+  <si>
+    <t>1643-03666</t>
+  </si>
+  <si>
+    <t>1313-80005</t>
+  </si>
+  <si>
+    <t>1313-45997</t>
+  </si>
+  <si>
+    <t>1643-03663</t>
+  </si>
+  <si>
+    <t>1313-35306</t>
+  </si>
+  <si>
+    <t>1643-03664</t>
+  </si>
+  <si>
+    <t>1313-80068</t>
+  </si>
+  <si>
+    <t>1643-03653</t>
+  </si>
+  <si>
+    <t>NO PINS</t>
+  </si>
+  <si>
+    <t>1643-03507</t>
+  </si>
+  <si>
+    <t>1643-03665</t>
+  </si>
+  <si>
+    <t>1313-46082</t>
+  </si>
+  <si>
+    <t>1643-03667</t>
+  </si>
+  <si>
+    <t>1313-80014</t>
+  </si>
+  <si>
+    <t>1313-90098</t>
+  </si>
+  <si>
+    <t>1643-10402</t>
+  </si>
+  <si>
+    <t>1643-03654</t>
+  </si>
+  <si>
+    <t>1643-03662</t>
+  </si>
+  <si>
+    <t>1313-90013</t>
+  </si>
+  <si>
+    <t>1313-46055</t>
+  </si>
+  <si>
+    <t>WEAKLING, MAYBE NHC</t>
+  </si>
+  <si>
+    <t>SCAV SHELL</t>
+  </si>
+  <si>
+    <t>1643-03661</t>
+  </si>
+  <si>
+    <t>1643-03660</t>
+  </si>
+  <si>
+    <t>1313-80043</t>
+  </si>
+  <si>
+    <t>1643-03659</t>
+  </si>
+  <si>
+    <t>1643-03658</t>
+  </si>
+  <si>
+    <t>1643-03657</t>
+  </si>
+  <si>
+    <t>1643-03570</t>
+  </si>
+  <si>
+    <t>1313-45911</t>
+  </si>
+  <si>
+    <t>1313-80100</t>
+  </si>
+  <si>
+    <t>1313-80051</t>
+  </si>
+  <si>
+    <t>1643-03656</t>
+  </si>
+  <si>
+    <t>1313-90073</t>
+  </si>
+  <si>
+    <t>1313-46000</t>
+  </si>
+  <si>
+    <t>1643-03668</t>
+  </si>
+  <si>
+    <t>1643-03674</t>
+  </si>
+  <si>
+    <t>1313-37164</t>
+  </si>
+  <si>
+    <t>1643-10456</t>
+  </si>
+  <si>
+    <t>1313-80007</t>
+  </si>
+  <si>
+    <t>1313-45994</t>
+  </si>
+  <si>
+    <t>1643-03528</t>
+  </si>
+  <si>
+    <t>1313-70062</t>
+  </si>
+  <si>
+    <t>1643-03673</t>
+  </si>
+  <si>
+    <t>1643-03516</t>
+  </si>
+  <si>
+    <t>PUKED KRILL</t>
+  </si>
+  <si>
+    <t>1643-03672</t>
+  </si>
+  <si>
+    <t>1643-03671</t>
+  </si>
+  <si>
+    <t>1313-80021</t>
+  </si>
+  <si>
+    <t>1643-03532</t>
+  </si>
+  <si>
+    <t>1313-80088</t>
+  </si>
+  <si>
+    <t>1643-03675</t>
+  </si>
+  <si>
+    <t>1313-80093</t>
+  </si>
+  <si>
+    <t>1643-03670</t>
+  </si>
+  <si>
+    <t>MUST HAVE LOST EGG</t>
   </si>
 </sst>
 </file>
@@ -626,7 +794,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -713,6 +881,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -995,11 +1164,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y174"/>
+  <dimension ref="A1:Y276"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A141" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G174" sqref="G174"/>
+      <pane ySplit="1" topLeftCell="A241" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L265" sqref="L265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7710,6 +7879,3040 @@
       </c>
       <c r="I174" s="15"/>
     </row>
+    <row r="175" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A175" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B175" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C175" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D175" s="17">
+        <v>1</v>
+      </c>
+      <c r="E175" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H175" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="176" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A176" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B176" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C176" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D176" s="17">
+        <v>2</v>
+      </c>
+      <c r="E176" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H176" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="177" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A177" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B177" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C177" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D177" s="17">
+        <v>3</v>
+      </c>
+      <c r="E177" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H177" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="178" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A178" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B178" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C178" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D178" s="17">
+        <v>4</v>
+      </c>
+      <c r="E178" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H178" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="179" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A179" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B179" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C179" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D179" s="17">
+        <v>5</v>
+      </c>
+      <c r="E179" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G179" t="s">
+        <v>37</v>
+      </c>
+      <c r="H179" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I179" t="s">
+        <v>166</v>
+      </c>
+      <c r="K179" t="s">
+        <v>112</v>
+      </c>
+      <c r="L179">
+        <v>10.25</v>
+      </c>
+      <c r="M179">
+        <v>118</v>
+      </c>
+      <c r="O179">
+        <v>173</v>
+      </c>
+      <c r="P179">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="180" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A180" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B180" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C180" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D180" s="17">
+        <v>6</v>
+      </c>
+      <c r="E180" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H180" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="181" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A181" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B181" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C181" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D181" s="17">
+        <v>7</v>
+      </c>
+      <c r="E181" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G181" t="s">
+        <v>37</v>
+      </c>
+      <c r="H181" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I181" t="s">
+        <v>168</v>
+      </c>
+      <c r="O181">
+        <v>180</v>
+      </c>
+      <c r="P181">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="182" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A182" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B182" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C182" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D182" s="17">
+        <v>8</v>
+      </c>
+      <c r="E182" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H182" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="183" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A183" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B183" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C183" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D183" s="17">
+        <v>9</v>
+      </c>
+      <c r="E183" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G183" t="s">
+        <v>37</v>
+      </c>
+      <c r="H183" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I183" t="s">
+        <v>111</v>
+      </c>
+      <c r="O183">
+        <v>190</v>
+      </c>
+      <c r="P183">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="184" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A184" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B184" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C184" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D184" s="17">
+        <v>10</v>
+      </c>
+      <c r="E184" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G184" t="s">
+        <v>37</v>
+      </c>
+      <c r="H184" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I184" t="s">
+        <v>114</v>
+      </c>
+      <c r="O184">
+        <v>170</v>
+      </c>
+      <c r="P184">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="185" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A185" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B185" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C185" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D185" s="17">
+        <v>11</v>
+      </c>
+      <c r="E185" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G185" t="s">
+        <v>26</v>
+      </c>
+      <c r="H185" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="M185">
+        <v>42</v>
+      </c>
+      <c r="N185">
+        <v>10</v>
+      </c>
+      <c r="O185">
+        <v>99</v>
+      </c>
+      <c r="P185">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="186" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A186" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B186" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C186" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D186" s="17">
+        <v>12</v>
+      </c>
+      <c r="E186" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G186" t="s">
+        <v>26</v>
+      </c>
+      <c r="H186" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I186" t="s">
+        <v>167</v>
+      </c>
+      <c r="M186">
+        <v>116</v>
+      </c>
+      <c r="N186">
+        <v>70</v>
+      </c>
+      <c r="O186">
+        <v>162</v>
+      </c>
+      <c r="P186">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="187" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A187" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B187" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C187" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D187" s="17">
+        <v>13</v>
+      </c>
+      <c r="E187" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G187" t="s">
+        <v>26</v>
+      </c>
+      <c r="H187" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M187">
+        <v>26</v>
+      </c>
+      <c r="O187">
+        <v>69</v>
+      </c>
+      <c r="P187">
+        <v>13</v>
+      </c>
+      <c r="U187" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="188" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A188" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B188" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C188" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D188" s="17">
+        <v>14</v>
+      </c>
+      <c r="E188" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G188" t="s">
+        <v>37</v>
+      </c>
+      <c r="H188" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I188" t="s">
+        <v>169</v>
+      </c>
+      <c r="O188">
+        <v>189</v>
+      </c>
+      <c r="P188">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="189" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A189" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B189" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C189" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D189" s="17">
+        <v>15</v>
+      </c>
+      <c r="E189" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H189" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="190" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A190" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B190" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C190" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D190" s="17">
+        <v>16</v>
+      </c>
+      <c r="E190" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H190" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="191" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A191" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B191" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C191" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D191" s="17">
+        <v>17</v>
+      </c>
+      <c r="E191" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H191" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="192" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A192" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B192" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C192" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D192" s="17">
+        <v>18</v>
+      </c>
+      <c r="E192" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H192" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="193" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A193" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B193" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C193" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D193" s="17">
+        <v>19</v>
+      </c>
+      <c r="E193" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G193" t="s">
+        <v>37</v>
+      </c>
+      <c r="H193" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I193" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="194" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A194" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B194" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C194" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D194" s="17">
+        <v>20</v>
+      </c>
+      <c r="E194" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G194" t="s">
+        <v>37</v>
+      </c>
+      <c r="H194" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I194" t="s">
+        <v>171</v>
+      </c>
+      <c r="O194">
+        <v>197</v>
+      </c>
+      <c r="P194">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="195" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A195" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B195" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C195" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D195" s="17">
+        <v>21</v>
+      </c>
+      <c r="E195" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G195" t="s">
+        <v>37</v>
+      </c>
+      <c r="H195" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I195" t="s">
+        <v>172</v>
+      </c>
+      <c r="M195">
+        <v>110</v>
+      </c>
+      <c r="N195">
+        <v>52</v>
+      </c>
+      <c r="O195">
+        <v>156</v>
+      </c>
+      <c r="P195">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="196" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A196" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B196" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C196" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D196" s="17">
+        <v>22</v>
+      </c>
+      <c r="E196" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H196" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="197" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A197" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B197" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C197" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D197" s="17">
+        <v>23</v>
+      </c>
+      <c r="E197" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G197" t="s">
+        <v>37</v>
+      </c>
+      <c r="H197" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I197" t="s">
+        <v>173</v>
+      </c>
+      <c r="O197">
+        <v>179</v>
+      </c>
+      <c r="P197">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="198" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A198" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B198" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C198" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D198" s="17">
+        <v>24</v>
+      </c>
+      <c r="E198" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G198" t="s">
+        <v>26</v>
+      </c>
+      <c r="H198" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I198" t="s">
+        <v>174</v>
+      </c>
+      <c r="M198">
+        <v>110</v>
+      </c>
+      <c r="N198">
+        <v>65</v>
+      </c>
+      <c r="O198">
+        <v>162</v>
+      </c>
+      <c r="P198">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="199" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A199" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B199" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C199" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D199" s="17">
+        <v>25</v>
+      </c>
+      <c r="E199" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H199" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="200" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A200" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B200" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C200" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D200" s="17">
+        <v>26</v>
+      </c>
+      <c r="E200" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H200" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="201" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A201" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B201" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C201" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D201" s="17">
+        <v>27</v>
+      </c>
+      <c r="E201" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G201" t="s">
+        <v>37</v>
+      </c>
+      <c r="H201" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I201" t="s">
+        <v>176</v>
+      </c>
+      <c r="O201">
+        <v>177</v>
+      </c>
+      <c r="P201">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="202" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A202" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B202" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C202" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D202" s="17">
+        <v>28</v>
+      </c>
+      <c r="E202" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G202" t="s">
+        <v>37</v>
+      </c>
+      <c r="H202" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I202" t="s">
+        <v>177</v>
+      </c>
+      <c r="K202" t="s">
+        <v>112</v>
+      </c>
+      <c r="L202">
+        <v>10</v>
+      </c>
+      <c r="M202">
+        <v>120</v>
+      </c>
+      <c r="O202">
+        <v>190</v>
+      </c>
+      <c r="P202">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="203" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A203" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B203" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C203" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D203" s="17">
+        <v>29</v>
+      </c>
+      <c r="E203" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G203" t="s">
+        <v>37</v>
+      </c>
+      <c r="H203" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I203" t="s">
+        <v>178</v>
+      </c>
+      <c r="O203">
+        <v>190</v>
+      </c>
+      <c r="P203">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="204" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A204" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B204" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C204" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D204" s="17">
+        <v>30</v>
+      </c>
+      <c r="E204" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H204" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="205" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A205" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B205" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C205" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D205" s="17">
+        <v>31</v>
+      </c>
+      <c r="E205" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G205" t="s">
+        <v>37</v>
+      </c>
+      <c r="H205" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I205" t="s">
+        <v>179</v>
+      </c>
+      <c r="K205" t="s">
+        <v>112</v>
+      </c>
+      <c r="L205">
+        <v>9</v>
+      </c>
+      <c r="M205">
+        <v>120</v>
+      </c>
+      <c r="O205">
+        <v>160</v>
+      </c>
+      <c r="P205">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="206" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A206" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B206" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C206" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D206" s="17">
+        <v>32</v>
+      </c>
+      <c r="E206" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G206" t="s">
+        <v>37</v>
+      </c>
+      <c r="H206" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I206" t="s">
+        <v>180</v>
+      </c>
+      <c r="O206">
+        <v>179</v>
+      </c>
+      <c r="P206">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="207" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A207" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B207" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C207" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D207" s="17">
+        <v>33</v>
+      </c>
+      <c r="E207" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H207" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="208" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A208" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B208" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C208" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D208" s="17">
+        <v>34</v>
+      </c>
+      <c r="E208" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H208" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="209" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A209" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B209" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C209" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D209" s="17">
+        <v>35</v>
+      </c>
+      <c r="E209" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H209" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="210" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A210" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B210" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C210" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D210" s="17">
+        <v>36</v>
+      </c>
+      <c r="E210" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H210" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="211" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A211" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B211" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C211" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D211" s="17">
+        <v>37</v>
+      </c>
+      <c r="E211" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G211" t="s">
+        <v>37</v>
+      </c>
+      <c r="H211" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I211" t="s">
+        <v>181</v>
+      </c>
+      <c r="O211">
+        <v>188</v>
+      </c>
+      <c r="P211">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="212" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A212" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B212" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C212" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D212" s="17">
+        <v>38</v>
+      </c>
+      <c r="E212" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G212" t="s">
+        <v>37</v>
+      </c>
+      <c r="H212" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I212" t="s">
+        <v>182</v>
+      </c>
+      <c r="O212">
+        <v>168</v>
+      </c>
+      <c r="P212">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="213" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A213" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B213" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C213" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D213" s="17">
+        <v>39</v>
+      </c>
+      <c r="E213" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G213" t="s">
+        <v>26</v>
+      </c>
+      <c r="H213" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O213">
+        <v>18</v>
+      </c>
+      <c r="P213">
+        <v>3</v>
+      </c>
+      <c r="U213" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="214" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A214" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B214" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C214" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D214" s="17">
+        <v>40</v>
+      </c>
+      <c r="E214" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H214" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="215" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A215" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B215" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C215" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D215" s="17">
+        <v>41</v>
+      </c>
+      <c r="E215" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G215" t="s">
+        <v>26</v>
+      </c>
+      <c r="H215" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I215" t="s">
+        <v>183</v>
+      </c>
+      <c r="M215">
+        <v>106</v>
+      </c>
+      <c r="N215">
+        <v>55</v>
+      </c>
+      <c r="O215">
+        <v>136</v>
+      </c>
+      <c r="P215">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="216" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A216" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B216" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C216" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D216" s="17">
+        <v>42</v>
+      </c>
+      <c r="E216" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H216" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="217" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A217" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B217" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C217" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D217" s="17">
+        <v>43</v>
+      </c>
+      <c r="E217" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G217" t="s">
+        <v>37</v>
+      </c>
+      <c r="H217" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I217" t="s">
+        <v>184</v>
+      </c>
+      <c r="K217" t="s">
+        <v>112</v>
+      </c>
+      <c r="L217">
+        <v>8.85</v>
+      </c>
+      <c r="M217">
+        <v>122</v>
+      </c>
+      <c r="O217">
+        <v>187</v>
+      </c>
+      <c r="P217">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="218" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A218" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B218" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C218" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D218" s="17">
+        <v>45</v>
+      </c>
+      <c r="E218" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H218" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="219" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A219" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B219" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C219" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D219" s="17">
+        <v>46</v>
+      </c>
+      <c r="E219" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G219" t="s">
+        <v>37</v>
+      </c>
+      <c r="H219" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I219" t="s">
+        <v>185</v>
+      </c>
+      <c r="O219">
+        <v>188</v>
+      </c>
+      <c r="P219">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="220" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A220" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B220" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C220" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D220" s="17">
+        <v>47</v>
+      </c>
+      <c r="E220" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G220" t="s">
+        <v>26</v>
+      </c>
+      <c r="H220" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="M220">
+        <v>52</v>
+      </c>
+      <c r="N220">
+        <v>15</v>
+      </c>
+      <c r="O220">
+        <v>110</v>
+      </c>
+      <c r="P220">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="221" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A221" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B221" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C221" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D221" s="17">
+        <v>48</v>
+      </c>
+      <c r="E221" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G221" t="s">
+        <v>37</v>
+      </c>
+      <c r="H221" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I221" t="s">
+        <v>186</v>
+      </c>
+      <c r="O221">
+        <v>179</v>
+      </c>
+      <c r="P221">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="222" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A222" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B222" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C222" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D222" s="17">
+        <v>1</v>
+      </c>
+      <c r="E222" t="s">
+        <v>59</v>
+      </c>
+      <c r="H222" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="223" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A223" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B223" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C223" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D223" s="17">
+        <v>2</v>
+      </c>
+      <c r="E223" t="s">
+        <v>59</v>
+      </c>
+      <c r="H223" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="U223" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="224" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A224" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B224" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C224" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D224" s="17">
+        <v>3</v>
+      </c>
+      <c r="E224" t="s">
+        <v>59</v>
+      </c>
+      <c r="H224" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="225" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A225" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B225" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C225" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D225" s="17">
+        <v>4</v>
+      </c>
+      <c r="E225" t="s">
+        <v>59</v>
+      </c>
+      <c r="H225" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="U225" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="226" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A226" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B226" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C226" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D226" s="17">
+        <v>5</v>
+      </c>
+      <c r="E226" t="s">
+        <v>59</v>
+      </c>
+      <c r="H226" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="227" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A227" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B227" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C227" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D227" s="17">
+        <v>6</v>
+      </c>
+      <c r="E227" t="s">
+        <v>59</v>
+      </c>
+      <c r="G227" t="s">
+        <v>37</v>
+      </c>
+      <c r="H227" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I227" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="O227">
+        <v>186</v>
+      </c>
+      <c r="P227">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="228" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A228" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B228" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C228" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D228" s="17">
+        <v>7</v>
+      </c>
+      <c r="E228" t="s">
+        <v>59</v>
+      </c>
+      <c r="G228" t="s">
+        <v>26</v>
+      </c>
+      <c r="H228" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I228" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="M228">
+        <v>120</v>
+      </c>
+      <c r="N228">
+        <v>65</v>
+      </c>
+      <c r="O228">
+        <v>154</v>
+      </c>
+      <c r="P228">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="229" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A229" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B229" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C229" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D229" s="17">
+        <v>8</v>
+      </c>
+      <c r="E229" t="s">
+        <v>59</v>
+      </c>
+      <c r="H229" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="230" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A230" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B230" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C230" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D230" s="17">
+        <v>9</v>
+      </c>
+      <c r="E230" t="s">
+        <v>59</v>
+      </c>
+      <c r="H230" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="231" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A231" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B231" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C231" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D231" s="17">
+        <v>10</v>
+      </c>
+      <c r="E231" t="s">
+        <v>59</v>
+      </c>
+      <c r="H231" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="232" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A232" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B232" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C232" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D232" s="17">
+        <v>11</v>
+      </c>
+      <c r="E232" t="s">
+        <v>59</v>
+      </c>
+      <c r="G232" t="s">
+        <v>26</v>
+      </c>
+      <c r="H232" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="M232">
+        <v>56</v>
+      </c>
+      <c r="N232">
+        <v>16</v>
+      </c>
+      <c r="O232">
+        <v>101</v>
+      </c>
+      <c r="P232">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="233" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A233" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B233" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C233" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D233" s="17">
+        <v>12</v>
+      </c>
+      <c r="E233" t="s">
+        <v>59</v>
+      </c>
+      <c r="G233" t="s">
+        <v>37</v>
+      </c>
+      <c r="H233" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I233" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K233" t="s">
+        <v>116</v>
+      </c>
+      <c r="L233">
+        <v>10.1</v>
+      </c>
+      <c r="M233">
+        <v>122</v>
+      </c>
+      <c r="O233">
+        <v>179</v>
+      </c>
+      <c r="P233">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="234" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A234" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B234" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C234" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D234" s="17">
+        <v>13</v>
+      </c>
+      <c r="E234" t="s">
+        <v>59</v>
+      </c>
+      <c r="G234" t="s">
+        <v>37</v>
+      </c>
+      <c r="H234" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I234" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="O234">
+        <v>184</v>
+      </c>
+      <c r="P234">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="235" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A235" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B235" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C235" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D235" s="17">
+        <v>14</v>
+      </c>
+      <c r="E235" t="s">
+        <v>59</v>
+      </c>
+      <c r="H235" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="236" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A236" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B236" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C236" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D236" s="17">
+        <v>15</v>
+      </c>
+      <c r="E236" t="s">
+        <v>59</v>
+      </c>
+      <c r="H236" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="237" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A237" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B237" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C237" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D237" s="17">
+        <v>16</v>
+      </c>
+      <c r="E237" t="s">
+        <v>59</v>
+      </c>
+      <c r="G237" t="s">
+        <v>37</v>
+      </c>
+      <c r="H237" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I237" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="M237">
+        <v>120</v>
+      </c>
+      <c r="O237">
+        <v>176</v>
+      </c>
+      <c r="P237">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="238" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A238" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B238" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C238" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D238" s="17">
+        <v>17</v>
+      </c>
+      <c r="E238" t="s">
+        <v>59</v>
+      </c>
+      <c r="G238" t="s">
+        <v>37</v>
+      </c>
+      <c r="H238" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I238" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="K238" t="s">
+        <v>112</v>
+      </c>
+      <c r="L238">
+        <v>10.25</v>
+      </c>
+      <c r="M238">
+        <v>122</v>
+      </c>
+      <c r="O238">
+        <v>195</v>
+      </c>
+      <c r="P238">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="239" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A239" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B239" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C239" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D239" s="17">
+        <v>18</v>
+      </c>
+      <c r="E239" t="s">
+        <v>59</v>
+      </c>
+      <c r="G239" t="s">
+        <v>37</v>
+      </c>
+      <c r="H239" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I239" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="K239" t="s">
+        <v>118</v>
+      </c>
+      <c r="L239">
+        <v>9.9</v>
+      </c>
+      <c r="M239">
+        <v>123</v>
+      </c>
+      <c r="O239">
+        <v>189</v>
+      </c>
+      <c r="P239">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="240" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A240" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B240" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C240" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D240" s="17">
+        <v>19</v>
+      </c>
+      <c r="E240" t="s">
+        <v>59</v>
+      </c>
+      <c r="G240" t="s">
+        <v>37</v>
+      </c>
+      <c r="H240" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I240" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="K240" t="s">
+        <v>118</v>
+      </c>
+      <c r="L240">
+        <v>8.85</v>
+      </c>
+      <c r="M240">
+        <v>123</v>
+      </c>
+      <c r="O240">
+        <v>171</v>
+      </c>
+      <c r="P240">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="241" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A241" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B241" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C241" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D241" s="17">
+        <v>20</v>
+      </c>
+      <c r="E241" t="s">
+        <v>59</v>
+      </c>
+      <c r="G241" t="s">
+        <v>37</v>
+      </c>
+      <c r="H241" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I241" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="O241">
+        <v>168</v>
+      </c>
+      <c r="P241">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="242" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A242" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B242" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C242" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D242" s="17">
+        <v>21</v>
+      </c>
+      <c r="E242" t="s">
+        <v>59</v>
+      </c>
+      <c r="H242" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="243" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A243" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B243" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C243" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D243" s="17">
+        <v>22</v>
+      </c>
+      <c r="E243" t="s">
+        <v>59</v>
+      </c>
+      <c r="H243" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="244" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A244" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B244" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C244" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D244" s="17">
+        <v>23</v>
+      </c>
+      <c r="E244" t="s">
+        <v>59</v>
+      </c>
+      <c r="G244" t="s">
+        <v>37</v>
+      </c>
+      <c r="H244" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I244" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="O244">
+        <v>179</v>
+      </c>
+      <c r="P244">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="245" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A245" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B245" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C245" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D245" s="17">
+        <v>24</v>
+      </c>
+      <c r="E245" t="s">
+        <v>59</v>
+      </c>
+      <c r="G245" t="s">
+        <v>37</v>
+      </c>
+      <c r="H245" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I245" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="O245">
+        <v>185</v>
+      </c>
+      <c r="P245">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="246" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A246" s="37">
+        <v>42525</v>
+      </c>
+      <c r="B246" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C246" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D246" s="17">
+        <v>25</v>
+      </c>
+      <c r="E246" t="s">
+        <v>59</v>
+      </c>
+      <c r="G246" t="s">
+        <v>37</v>
+      </c>
+      <c r="H246" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I246" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="K246" t="s">
+        <v>118</v>
+      </c>
+      <c r="L246">
+        <v>10.5</v>
+      </c>
+      <c r="M246">
+        <v>124</v>
+      </c>
+      <c r="O246">
+        <v>177</v>
+      </c>
+      <c r="P246">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="247" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A247" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B247" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C247" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D247" s="17">
+        <v>5</v>
+      </c>
+      <c r="E247" t="s">
+        <v>22</v>
+      </c>
+      <c r="G247" t="s">
+        <v>37</v>
+      </c>
+      <c r="H247" t="s">
+        <v>38</v>
+      </c>
+      <c r="I247" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="K247" t="s">
+        <v>118</v>
+      </c>
+      <c r="L247">
+        <v>8.75</v>
+      </c>
+      <c r="M247">
+        <v>124</v>
+      </c>
+      <c r="O247">
+        <v>181</v>
+      </c>
+      <c r="P247">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="248" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A248" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B248" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C248" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D248" s="17">
+        <v>7</v>
+      </c>
+      <c r="E248" t="s">
+        <v>22</v>
+      </c>
+      <c r="G248" t="s">
+        <v>37</v>
+      </c>
+      <c r="H248" t="s">
+        <v>38</v>
+      </c>
+      <c r="I248" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="M248">
+        <v>123</v>
+      </c>
+      <c r="O248">
+        <v>181</v>
+      </c>
+      <c r="P248">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="249" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A249" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B249" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C249" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D249" s="17">
+        <v>9</v>
+      </c>
+      <c r="E249" t="s">
+        <v>22</v>
+      </c>
+      <c r="G249" t="s">
+        <v>37</v>
+      </c>
+      <c r="H249" t="s">
+        <v>38</v>
+      </c>
+      <c r="I249" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="M249">
+        <v>124</v>
+      </c>
+      <c r="O249">
+        <v>199</v>
+      </c>
+      <c r="P249">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="250" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A250" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B250" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C250" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D250" s="17">
+        <v>10</v>
+      </c>
+      <c r="E250" t="s">
+        <v>22</v>
+      </c>
+      <c r="G250" t="s">
+        <v>37</v>
+      </c>
+      <c r="H250" t="s">
+        <v>38</v>
+      </c>
+      <c r="I250" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="K250" t="s">
+        <v>116</v>
+      </c>
+      <c r="L250">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="M250">
+        <v>123</v>
+      </c>
+      <c r="O250">
+        <v>178.5</v>
+      </c>
+      <c r="P250">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="251" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A251" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B251" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C251" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D251" s="17">
+        <v>14</v>
+      </c>
+      <c r="E251" t="s">
+        <v>22</v>
+      </c>
+      <c r="G251" t="s">
+        <v>37</v>
+      </c>
+      <c r="H251" t="s">
+        <v>38</v>
+      </c>
+      <c r="I251" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="K251" t="s">
+        <v>112</v>
+      </c>
+      <c r="L251">
+        <v>10.5</v>
+      </c>
+      <c r="M251">
+        <v>124</v>
+      </c>
+      <c r="O251">
+        <v>185</v>
+      </c>
+      <c r="P251">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="252" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A252" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B252" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C252" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D252" s="17">
+        <v>19</v>
+      </c>
+      <c r="E252" t="s">
+        <v>22</v>
+      </c>
+      <c r="G252" t="s">
+        <v>37</v>
+      </c>
+      <c r="H252" t="s">
+        <v>38</v>
+      </c>
+      <c r="I252" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="M252">
+        <v>130</v>
+      </c>
+      <c r="O252">
+        <v>183</v>
+      </c>
+      <c r="P252">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="253" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A253" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B253" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C253" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D253" s="17">
+        <v>23</v>
+      </c>
+      <c r="E253" t="s">
+        <v>22</v>
+      </c>
+      <c r="G253" t="s">
+        <v>37</v>
+      </c>
+      <c r="H253" t="s">
+        <v>38</v>
+      </c>
+      <c r="I253" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="M253">
+        <v>121</v>
+      </c>
+      <c r="O253">
+        <v>187</v>
+      </c>
+      <c r="P253">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="254" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A254" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B254" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C254" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D254" s="17">
+        <v>27</v>
+      </c>
+      <c r="E254" t="s">
+        <v>22</v>
+      </c>
+      <c r="G254" t="s">
+        <v>37</v>
+      </c>
+      <c r="H254" t="s">
+        <v>38</v>
+      </c>
+      <c r="I254" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="M254">
+        <v>124</v>
+      </c>
+      <c r="O254">
+        <v>183</v>
+      </c>
+      <c r="P254">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="255" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A255" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B255" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C255" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D255" s="17">
+        <v>28</v>
+      </c>
+      <c r="E255" t="s">
+        <v>22</v>
+      </c>
+      <c r="G255" t="s">
+        <v>37</v>
+      </c>
+      <c r="H255" t="s">
+        <v>38</v>
+      </c>
+      <c r="I255" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="M255">
+        <v>123</v>
+      </c>
+      <c r="O255">
+        <v>163</v>
+      </c>
+      <c r="P255">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="256" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A256" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B256" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C256" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D256" s="17">
+        <v>31</v>
+      </c>
+      <c r="E256" t="s">
+        <v>22</v>
+      </c>
+      <c r="G256" t="s">
+        <v>37</v>
+      </c>
+      <c r="H256" t="s">
+        <v>38</v>
+      </c>
+      <c r="I256" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="M256">
+        <v>127</v>
+      </c>
+      <c r="O256">
+        <v>173</v>
+      </c>
+      <c r="P256">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="257" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A257" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B257" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C257" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D257" s="17">
+        <v>32</v>
+      </c>
+      <c r="E257" t="s">
+        <v>22</v>
+      </c>
+      <c r="G257" t="s">
+        <v>37</v>
+      </c>
+      <c r="H257" t="s">
+        <v>38</v>
+      </c>
+      <c r="I257" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="M257">
+        <v>124</v>
+      </c>
+      <c r="O257">
+        <v>193</v>
+      </c>
+      <c r="P257">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="258" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A258" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B258" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C258" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D258" s="17">
+        <v>37</v>
+      </c>
+      <c r="E258" t="s">
+        <v>22</v>
+      </c>
+      <c r="G258" t="s">
+        <v>37</v>
+      </c>
+      <c r="H258" t="s">
+        <v>38</v>
+      </c>
+      <c r="I258" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="M258">
+        <v>125</v>
+      </c>
+      <c r="O258">
+        <v>197</v>
+      </c>
+      <c r="P258">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="259" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A259" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B259" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C259" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D259" s="17">
+        <v>38</v>
+      </c>
+      <c r="E259" t="s">
+        <v>22</v>
+      </c>
+      <c r="G259" t="s">
+        <v>37</v>
+      </c>
+      <c r="H259" t="s">
+        <v>38</v>
+      </c>
+      <c r="I259" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="M259">
+        <v>126</v>
+      </c>
+      <c r="O259">
+        <v>194</v>
+      </c>
+      <c r="P259">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="260" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A260" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B260" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C260" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D260" s="17">
+        <v>43</v>
+      </c>
+      <c r="E260" t="s">
+        <v>22</v>
+      </c>
+      <c r="G260" t="s">
+        <v>37</v>
+      </c>
+      <c r="H260" t="s">
+        <v>55</v>
+      </c>
+      <c r="I260" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="U260" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="261" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A261" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B261" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C261" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D261" s="17">
+        <v>46</v>
+      </c>
+      <c r="E261" t="s">
+        <v>22</v>
+      </c>
+      <c r="G261" t="s">
+        <v>37</v>
+      </c>
+      <c r="H261" t="s">
+        <v>38</v>
+      </c>
+      <c r="I261" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="K261" t="s">
+        <v>116</v>
+      </c>
+      <c r="L261">
+        <v>10.25</v>
+      </c>
+      <c r="M261">
+        <v>122</v>
+      </c>
+      <c r="O261">
+        <v>188</v>
+      </c>
+      <c r="P261">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="262" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A262" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B262" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C262" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D262" s="17">
+        <v>48</v>
+      </c>
+      <c r="E262" t="s">
+        <v>22</v>
+      </c>
+      <c r="G262" t="s">
+        <v>37</v>
+      </c>
+      <c r="H262" t="s">
+        <v>38</v>
+      </c>
+      <c r="I262" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="M262">
+        <v>126</v>
+      </c>
+      <c r="O262">
+        <v>184</v>
+      </c>
+      <c r="P262">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="263" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A263" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B263" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C263" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D263" s="17">
+        <v>6</v>
+      </c>
+      <c r="E263" t="s">
+        <v>59</v>
+      </c>
+      <c r="G263" t="s">
+        <v>37</v>
+      </c>
+      <c r="H263" t="s">
+        <v>38</v>
+      </c>
+      <c r="I263" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="K263" t="s">
+        <v>118</v>
+      </c>
+      <c r="L263">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="M263">
+        <v>121</v>
+      </c>
+      <c r="O263">
+        <v>168</v>
+      </c>
+      <c r="P263">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="264" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A264" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B264" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C264" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D264" s="17">
+        <v>12</v>
+      </c>
+      <c r="E264" t="s">
+        <v>59</v>
+      </c>
+      <c r="G264" t="s">
+        <v>37</v>
+      </c>
+      <c r="H264" t="s">
+        <v>38</v>
+      </c>
+      <c r="I264" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="K264" t="s">
+        <v>118</v>
+      </c>
+      <c r="L264">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="M264">
+        <v>120</v>
+      </c>
+      <c r="O264">
+        <v>173</v>
+      </c>
+      <c r="P264">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="265" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A265" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B265" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C265" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D265" s="17">
+        <v>13</v>
+      </c>
+      <c r="E265" t="s">
+        <v>59</v>
+      </c>
+      <c r="G265" t="s">
+        <v>37</v>
+      </c>
+      <c r="H265" t="s">
+        <v>38</v>
+      </c>
+      <c r="I265" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="M265">
+        <v>121</v>
+      </c>
+      <c r="O265">
+        <v>181</v>
+      </c>
+      <c r="P265">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="266" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A266" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B266" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C266" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D266" s="17">
+        <v>16</v>
+      </c>
+      <c r="E266" t="s">
+        <v>59</v>
+      </c>
+      <c r="G266" t="s">
+        <v>37</v>
+      </c>
+      <c r="H266" t="s">
+        <v>38</v>
+      </c>
+      <c r="I266" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="M266">
+        <v>127</v>
+      </c>
+      <c r="O266">
+        <v>189</v>
+      </c>
+      <c r="P266">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="267" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A267" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B267" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C267" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D267" s="17">
+        <v>17</v>
+      </c>
+      <c r="E267" t="s">
+        <v>59</v>
+      </c>
+      <c r="G267" t="s">
+        <v>37</v>
+      </c>
+      <c r="H267" t="s">
+        <v>38</v>
+      </c>
+      <c r="I267" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="M267">
+        <v>126</v>
+      </c>
+      <c r="O267">
+        <v>190</v>
+      </c>
+      <c r="P267">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="268" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A268" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B268" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C268" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D268" s="17">
+        <v>18</v>
+      </c>
+      <c r="E268" t="s">
+        <v>59</v>
+      </c>
+      <c r="G268" t="s">
+        <v>37</v>
+      </c>
+      <c r="H268" t="s">
+        <v>38</v>
+      </c>
+      <c r="I268" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="M268">
+        <v>124</v>
+      </c>
+      <c r="O268">
+        <v>186</v>
+      </c>
+      <c r="P268">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="269" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A269" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B269" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C269" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D269" s="17">
+        <v>19</v>
+      </c>
+      <c r="E269" t="s">
+        <v>59</v>
+      </c>
+      <c r="G269" t="s">
+        <v>37</v>
+      </c>
+      <c r="H269" t="s">
+        <v>38</v>
+      </c>
+      <c r="I269" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="M269">
+        <v>119</v>
+      </c>
+      <c r="O269">
+        <v>178</v>
+      </c>
+      <c r="P269">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="270" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A270" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B270" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C270" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D270" s="17">
+        <v>20</v>
+      </c>
+      <c r="E270" t="s">
+        <v>59</v>
+      </c>
+      <c r="G270" t="s">
+        <v>37</v>
+      </c>
+      <c r="H270" t="s">
+        <v>38</v>
+      </c>
+      <c r="I270" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="K270" t="s">
+        <v>112</v>
+      </c>
+      <c r="L270">
+        <v>10.8</v>
+      </c>
+      <c r="M270">
+        <v>125</v>
+      </c>
+      <c r="O270">
+        <v>204</v>
+      </c>
+      <c r="P270">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="271" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A271" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B271" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C271" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D271" s="17">
+        <v>23</v>
+      </c>
+      <c r="E271" t="s">
+        <v>59</v>
+      </c>
+      <c r="G271" t="s">
+        <v>37</v>
+      </c>
+      <c r="H271" t="s">
+        <v>38</v>
+      </c>
+      <c r="I271" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="M271">
+        <v>126</v>
+      </c>
+      <c r="O271">
+        <v>172</v>
+      </c>
+      <c r="P271">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="272" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A272" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B272" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C272" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D272" s="17">
+        <v>24</v>
+      </c>
+      <c r="E272" t="s">
+        <v>59</v>
+      </c>
+      <c r="G272" t="s">
+        <v>37</v>
+      </c>
+      <c r="H272" t="s">
+        <v>23</v>
+      </c>
+      <c r="I272" s="15"/>
+      <c r="U272" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="273" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A273" s="37">
+        <v>42526</v>
+      </c>
+      <c r="B273" s="38">
+        <v>2016</v>
+      </c>
+      <c r="C273" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D273" s="17">
+        <v>25</v>
+      </c>
+      <c r="E273" t="s">
+        <v>59</v>
+      </c>
+      <c r="G273" t="s">
+        <v>37</v>
+      </c>
+      <c r="H273" t="s">
+        <v>38</v>
+      </c>
+      <c r="I273" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="K273" t="s">
+        <v>112</v>
+      </c>
+      <c r="L273">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="M273">
+        <v>127</v>
+      </c>
+      <c r="O273">
+        <v>178</v>
+      </c>
+      <c r="P273">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="274" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A274" s="37"/>
+      <c r="B274" s="38"/>
+      <c r="C274" s="42"/>
+      <c r="D274" s="17"/>
+      <c r="I274" s="15"/>
+    </row>
+    <row r="275" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A275" s="37"/>
+      <c r="B275" s="38"/>
+      <c r="C275" s="42"/>
+      <c r="D275" s="17"/>
+      <c r="I275" s="15"/>
+    </row>
+    <row r="276" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A276" s="37"/>
+      <c r="B276" s="38"/>
+      <c r="C276" s="42"/>
+      <c r="D276" s="17"/>
+      <c r="I276" s="15"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7720,7 +10923,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>